<commit_message>
Fix board/bom errors from initial build
* Accelerometer (U501) footprint mirrored. Redraw footprint and adjust routing.
* Gyro (U505) footprint mirrored. Redraw footprint and adjust routing.
* Codec (U702) labed as wrong chip. Says WM8731 but should be 8750. Also fix in BOM.
* Should include OLED screen in BOM (not just the connector).
* Codec to TRRS caps have incorrect value. Says 220uF but should be 220pF.
* Mark RPi Hat EEPROM circuit as depopulated in schematic.
* Remove dangling trace near encoder headers.
</commit_message>
<xml_diff>
--- a/pcb/labio.bom.xlsx
+++ b/pcb/labio.bom.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="251">
   <si>
     <t>Source</t>
   </si>
@@ -44,15 +44,6 @@
     <t>Generated Date</t>
   </si>
   <si>
-    <t>Monday</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> July 25</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2016 'PMt' 11:51:32 PM</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -281,9 +272,6 @@
     <t>U702</t>
   </si>
   <si>
-    <t>WM8731</t>
-  </si>
-  <si>
     <t>Housings_DFN_QFN:QFN-32-1EP_5x5mm_Pitch0.5mm</t>
   </si>
   <si>
@@ -443,9 +431,6 @@
     <t>D301, D501, D601, D602, D603, D604, D605, D606, D607, D608, D609, D610, D614, D615, D616, D617, D627, D628, D701</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>P601, P602, P604</t>
   </si>
   <si>
@@ -548,18 +533,6 @@
     <t>Cirrus Logic</t>
   </si>
   <si>
-    <t>WM8731CLSEFL/R</t>
-  </si>
-  <si>
-    <t>IC CODEC PORTABLE INTERNET 28QFN</t>
-  </si>
-  <si>
-    <t>WM8731CLSEFL/RCT-ND</t>
-  </si>
-  <si>
-    <t>http://www.digikey.com/product-detail/en/cirrus-logic-inc/WM8731CLSEFL-R/WM8731CLSEFL-RCT-ND/5036759</t>
-  </si>
-  <si>
     <t>TI</t>
   </si>
   <si>
@@ -759,6 +732,54 @@
   </si>
   <si>
     <t>Board Mount Pressure Sensors Digital Barometer 2.7uA, 300-1200hPa</t>
+  </si>
+  <si>
+    <t>Monday July 25 2016 'PMt' 11:51:32 PM</t>
+  </si>
+  <si>
+    <t>WM8750</t>
+  </si>
+  <si>
+    <t>U401</t>
+  </si>
+  <si>
+    <t>WM8750CJLGEFL</t>
+  </si>
+  <si>
+    <t>IC CODEC STEREO PORTABLE 32QFN</t>
+  </si>
+  <si>
+    <t>598-2392-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/cirrus-logic-inc/WM8750CJLGEFL/598-2392-ND/5409917</t>
+  </si>
+  <si>
+    <t>CFAL12832D-B</t>
+  </si>
+  <si>
+    <t>Crystalfontz</t>
+  </si>
+  <si>
+    <t>128x32 I2C Graphic OLED - ZIF</t>
+  </si>
+  <si>
+    <t>https://www.crystalfontz.com/product/cfal12832db-graphic-128x32-oled</t>
+  </si>
+  <si>
+    <t>Bourns</t>
+  </si>
+  <si>
+    <t>PEC12R-4220F-N0024</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12 mm Incremental Encoder </t>
+  </si>
+  <si>
+    <t>PEC12R-4220F-N0024-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/bourns-inc/PEC12R-4220F-N0024/PEC12R-4220F-N0024-ND/4499652</t>
   </si>
 </sst>
 </file>
@@ -1108,11 +1129,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G49" sqref="G49"/>
+      <pane ySplit="8" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I54" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1148,88 +1169,82 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
+        <v>235</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>160</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D9" s="5">
         <v>22</v>
@@ -1243,43 +1258,43 @@
     </row>
     <row r="10" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D10" s="5">
         <v>10</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D11" s="5">
         <v>1</v>
@@ -1293,43 +1308,43 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="D12" s="5">
         <v>4</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D13" s="5">
         <v>1</v>
@@ -1343,13 +1358,13 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D14" s="5">
         <v>3</v>
@@ -1363,13 +1378,13 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D15" s="5">
         <v>1</v>
@@ -1383,19 +1398,19 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D16" s="5">
         <v>5</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -1405,79 +1420,79 @@
     </row>
     <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D17" s="5">
         <v>19</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="I17" s="5" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D18" s="5">
         <v>12</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D19" s="5">
         <v>1</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -1487,19 +1502,19 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="D20" s="5">
         <v>1</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
@@ -1509,19 +1524,19 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D21" s="5">
         <v>1</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
@@ -1531,19 +1546,19 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D22" s="5">
         <v>1</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
@@ -1553,19 +1568,19 @@
     </row>
     <row r="23" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D23" s="5">
         <v>9</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -1575,19 +1590,19 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D24" s="5">
         <v>1</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -1597,43 +1612,43 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D25" s="5">
         <v>1</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="I25" s="5" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D26" s="5">
         <v>1</v>
@@ -1647,19 +1662,19 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D27" s="5">
         <v>7</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -1669,49 +1684,49 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D28" s="5">
         <v>1</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D29" s="5">
         <v>1</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
@@ -1721,19 +1736,19 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="D30" s="5">
         <v>2</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -1743,19 +1758,19 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D31" s="5">
         <v>2</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
@@ -1765,19 +1780,19 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="D32" s="5">
         <v>1</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
@@ -1787,19 +1802,19 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D33" s="5">
         <v>1</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
@@ -1809,73 +1824,73 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D34" s="5">
         <v>1</v>
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="H34" s="5" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="I34" s="5" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="J34" s="5" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D35" s="5">
         <v>15</v>
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="H35" s="5" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="I35" s="5" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D36" s="5">
         <v>2</v>
@@ -1889,19 +1904,19 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D37" s="5">
         <v>1</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
@@ -1911,13 +1926,13 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D38" s="5">
         <v>2</v>
@@ -1931,13 +1946,13 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D39" s="5">
         <v>1</v>
@@ -1951,13 +1966,13 @@
     </row>
     <row r="40" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B40" s="5">
         <v>220</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D40" s="5">
         <v>19</v>
@@ -1971,13 +1986,13 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D41" s="5">
         <v>2</v>
@@ -1991,13 +2006,13 @@
     </row>
     <row r="42" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B42" s="5">
         <v>0</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D42" s="5">
         <v>14</v>
@@ -2011,19 +2026,19 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D43" s="5">
         <v>3</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
@@ -2033,13 +2048,13 @@
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D44" s="5">
         <v>2</v>
@@ -2053,13 +2068,13 @@
     </row>
     <row r="45" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D45" s="5">
         <v>15</v>
@@ -2073,13 +2088,13 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B46" s="5">
         <v>0.01</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D46" s="5">
         <v>2</v>
@@ -2093,13 +2108,13 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D47" s="5">
         <v>1</v>
@@ -2113,13 +2128,13 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D48" s="5">
         <v>1</v>
@@ -2133,212 +2148,222 @@
     </row>
     <row r="49" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D49" s="5">
         <v>10</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>138</v>
+        <v>76</v>
+      </c>
+      <c r="D50" s="5">
+        <v>1</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
+        <v>130</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D51" s="5">
         <v>5</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="D52" s="5">
         <v>1</v>
       </c>
       <c r="E52" s="5"/>
       <c r="F52" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="H52" s="5" t="s">
         <v>156</v>
       </c>
-      <c r="G52" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>161</v>
-      </c>
       <c r="I52" s="5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D53" s="5">
         <v>1</v>
       </c>
       <c r="E53" s="5"/>
       <c r="F53" s="5" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>53</v>
+        <v>237</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C54" s="5" t="s">
-        <v>55</v>
-      </c>
+        <v>242</v>
+      </c>
+      <c r="C54" s="5"/>
       <c r="D54" s="5">
         <v>1</v>
       </c>
-      <c r="E54" s="5"/>
+      <c r="E54" s="5" t="s">
+        <v>130</v>
+      </c>
       <c r="F54" s="5" t="s">
-        <v>212</v>
+        <v>243</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>221</v>
+        <v>242</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>222</v>
+        <v>244</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>224</v>
+        <v>245</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D55" s="5">
         <v>1</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="5" t="s">
-        <v>225</v>
+        <v>203</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>57</v>
+        <v>212</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>243</v>
+        <v>213</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>242</v>
+        <v>214</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>241</v>
+        <v>215</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C56" s="5" t="s">
         <v>55</v>
@@ -2348,132 +2373,162 @@
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="5" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>217</v>
+        <v>54</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>219</v>
+        <v>233</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>82</v>
+        <v>52</v>
       </c>
       <c r="D57" s="5">
         <v>1</v>
       </c>
       <c r="E57" s="5"/>
       <c r="F57" s="5" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="D58" s="5">
         <v>1</v>
       </c>
       <c r="E58" s="5"/>
       <c r="F58" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="H58" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="I58" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="J58" s="5" t="s">
         <v>207</v>
-      </c>
-      <c r="G58" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="H58" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="I58" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="J58" s="5" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>85</v>
+        <v>89</v>
       </c>
       <c r="D59" s="5">
         <v>1</v>
       </c>
       <c r="E59" s="5"/>
       <c r="F59" s="5" t="s">
-        <v>172</v>
+        <v>198</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>173</v>
+        <v>199</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>174</v>
+        <v>201</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>175</v>
+        <v>200</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>176</v>
+        <v>202</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>25</v>
+        <v>236</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="D60" s="5">
+        <v>1</v>
+      </c>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D61" s="5">
         <v>2</v>
       </c>
-      <c r="E60" s="5" t="s">
-        <v>134</v>
-      </c>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
-      <c r="J60" s="5"/>
+      <c r="E61" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
     </row>
   </sheetData>
   <sortState ref="A9:J60">

</xml_diff>

<commit_message>
Power motor driver from 5V but with 3.3V logic. Adjust R601, R602 to prevent more than 3.3V on logic lines.
</commit_message>
<xml_diff>
--- a/pcb/labio.bom.xlsx
+++ b/pcb/labio.bom.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="980" yWindow="460" windowWidth="32620" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="460" windowWidth="32560" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="labio.bom" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="249">
   <si>
     <t>Source</t>
   </si>
@@ -248,9 +248,6 @@
     <t>20k</t>
   </si>
   <si>
-    <t>1k</t>
-  </si>
-  <si>
     <t>SW605</t>
   </si>
   <si>
@@ -446,9 +443,6 @@
     <t>R401, R402, R403, R502, R504, R505, R506, R507, R508, R509, R510, R511, R513, R515</t>
   </si>
   <si>
-    <t>R601, R602</t>
-  </si>
-  <si>
     <t>R603, R604, R608, R609, R610, R611, R616, R617, R620, R621, R625, R628, R629, R632, R633</t>
   </si>
   <si>
@@ -464,9 +458,6 @@
     <t>Q302, Q303, Q601, Q602, Q603, Q604, Q605, Q606, Q607, Q608, Q609, Q610, Q611, Q612, Q613</t>
   </si>
   <si>
-    <t>R303, R304</t>
-  </si>
-  <si>
     <t>dnp-10k</t>
   </si>
   <si>
@@ -780,6 +771,9 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/bourns-inc/PEC12R-4220F-N0024/PEC12R-4220F-N0024-ND/4499652</t>
+  </si>
+  <si>
+    <t>R303, R304, R601, R602</t>
   </si>
 </sst>
 </file>
@@ -1129,11 +1123,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J61"/>
+  <dimension ref="A1:J60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I54" sqref="I54"/>
+      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1169,7 +1163,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1215,30 +1209,30 @@
         <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>120</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>28</v>
@@ -1258,7 +1252,7 @@
     </row>
     <row r="10" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>48</v>
@@ -1271,19 +1265,19 @@
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="I10" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>228</v>
-      </c>
-      <c r="H10" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>230</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -1308,7 +1302,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>67</v>
@@ -1321,27 +1315,27 @@
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="I12" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="J12" s="5" t="s">
         <v>223</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>225</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>91</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>29</v>
@@ -1358,10 +1352,10 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>29</v>
@@ -1378,10 +1372,10 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>93</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>94</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>29</v>
@@ -1398,10 +1392,10 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>29</v>
@@ -1410,7 +1404,7 @@
         <v>5</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -1420,7 +1414,7 @@
     </row>
     <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>42</v>
@@ -1433,24 +1427,24 @@
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="I17" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="J17" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>195</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>196</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>197</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>69</v>
@@ -1463,36 +1457,36 @@
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="I18" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="J18" s="5" t="s">
         <v>158</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="B19" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="C19" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>114</v>
-      </c>
       <c r="D19" s="5">
         <v>1</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -1502,19 +1496,19 @@
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="B20" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C20" s="5" t="s">
-        <v>109</v>
-      </c>
       <c r="D20" s="5">
         <v>1</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F20" s="5"/>
       <c r="G20" s="5"/>
@@ -1524,19 +1518,19 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>116</v>
-      </c>
       <c r="D21" s="5">
         <v>1</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
@@ -1546,19 +1540,19 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C22" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>111</v>
-      </c>
       <c r="D22" s="5">
         <v>1</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F22" s="5"/>
       <c r="G22" s="5"/>
@@ -1568,19 +1562,19 @@
     </row>
     <row r="23" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B23" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C23" s="5" t="s">
         <v>105</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>106</v>
       </c>
       <c r="D23" s="5">
         <v>9</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -1602,7 +1596,7 @@
         <v>1</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -1612,32 +1606,32 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>85</v>
-      </c>
-      <c r="C25" s="5" t="s">
-        <v>86</v>
       </c>
       <c r="D25" s="5">
         <v>1</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I25" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="J25" s="5" t="s">
         <v>179</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -1662,7 +1656,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>33</v>
@@ -1674,7 +1668,7 @@
         <v>7</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -1697,24 +1691,24 @@
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="I28" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="G28" s="5" t="s">
+      <c r="J28" s="5" t="s">
         <v>189</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>65</v>
@@ -1726,7 +1720,7 @@
         <v>1</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
@@ -1736,7 +1730,7 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B30" s="5" t="s">
         <v>61</v>
@@ -1748,7 +1742,7 @@
         <v>2</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -1758,7 +1752,7 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B31" s="5" t="s">
         <v>63</v>
@@ -1770,7 +1764,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
@@ -1780,19 +1774,19 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>65</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D32" s="5">
         <v>1</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
@@ -1802,19 +1796,19 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="C33" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>104</v>
-      </c>
       <c r="D33" s="5">
         <v>1</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
@@ -1837,24 +1831,24 @@
       </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="I34" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="J34" s="5" t="s">
         <v>174</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B35" s="5" t="s">
         <v>43</v>
@@ -1867,24 +1861,24 @@
       </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="I35" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="J35" s="5" t="s">
         <v>218</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>219</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B36" s="5" t="s">
         <v>24</v>
@@ -1907,7 +1901,7 @@
         <v>19</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C37" s="5" t="s">
         <v>21</v>
@@ -1916,7 +1910,7 @@
         <v>1</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
@@ -1926,10 +1920,10 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C38" s="5" t="s">
         <v>21</v>
@@ -1966,7 +1960,7 @@
     </row>
     <row r="40" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B40" s="5">
         <v>220</v>
@@ -1986,7 +1980,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>145</v>
+        <v>248</v>
       </c>
       <c r="B41" s="5" t="s">
         <v>20</v>
@@ -1995,7 +1989,7 @@
         <v>21</v>
       </c>
       <c r="D41" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -2006,7 +2000,7 @@
     </row>
     <row r="42" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B42" s="5">
         <v>0</v>
@@ -2026,7 +2020,7 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B43" s="5" t="s">
         <v>56</v>
@@ -2038,7 +2032,7 @@
         <v>3</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
@@ -2046,18 +2040,18 @@
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D44" s="5">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
@@ -2066,18 +2060,18 @@
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>72</v>
+        <v>141</v>
+      </c>
+      <c r="B45" s="5">
+        <v>0.01</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="D45" s="5">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
@@ -2088,16 +2082,16 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>143</v>
-      </c>
-      <c r="B46" s="5">
-        <v>0.01</v>
+        <v>94</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>95</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="D46" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
@@ -2108,10 +2102,10 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>21</v>
@@ -2126,409 +2120,389 @@
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>97</v>
+        <v>130</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>98</v>
+        <v>40</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
       <c r="D48" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="5"/>
-      <c r="J48" s="5"/>
-    </row>
-    <row r="49" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="F48" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>131</v>
+        <v>73</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="D49" s="5">
-        <v>10</v>
-      </c>
-      <c r="E49" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>129</v>
+      </c>
       <c r="F49" s="5" t="s">
-        <v>183</v>
+        <v>243</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>184</v>
+        <v>244</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>185</v>
+        <v>245</v>
       </c>
       <c r="I49" s="5" t="s">
-        <v>186</v>
+        <v>246</v>
       </c>
       <c r="J49" s="5" t="s">
-        <v>187</v>
+        <v>247</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>75</v>
+        <v>98</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
       <c r="D50" s="5">
-        <v>1</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>130</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E50" s="5"/>
       <c r="F50" s="5" t="s">
-        <v>246</v>
+        <v>159</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>247</v>
+        <v>160</v>
       </c>
       <c r="H50" s="5" t="s">
-        <v>248</v>
+        <v>161</v>
       </c>
       <c r="I50" s="5" t="s">
-        <v>249</v>
+        <v>162</v>
       </c>
       <c r="J50" s="5" t="s">
-        <v>250</v>
+        <v>163</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>122</v>
+        <v>25</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>99</v>
+        <v>26</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>100</v>
+        <v>27</v>
       </c>
       <c r="D51" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>165</v>
+        <v>150</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>166</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
       <c r="D52" s="5">
         <v>1</v>
       </c>
       <c r="E52" s="5"/>
       <c r="F52" s="5" t="s">
-        <v>151</v>
+        <v>165</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>156</v>
+        <v>168</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>30</v>
+        <v>234</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="C53" s="5"/>
       <c r="D53" s="5">
         <v>1</v>
       </c>
-      <c r="E53" s="5"/>
+      <c r="E53" s="5" t="s">
+        <v>129</v>
+      </c>
       <c r="F53" s="5" t="s">
-        <v>168</v>
+        <v>240</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>169</v>
+        <v>239</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>171</v>
+        <v>241</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>170</v>
+        <v>230</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>172</v>
+        <v>242</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>237</v>
+        <v>50</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="C54" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="D54" s="5">
         <v>1</v>
       </c>
-      <c r="E54" s="5" t="s">
-        <v>130</v>
-      </c>
+      <c r="E54" s="5"/>
       <c r="F54" s="5" t="s">
-        <v>243</v>
+        <v>200</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>242</v>
+        <v>209</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>244</v>
+        <v>210</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>233</v>
+        <v>211</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>245</v>
+        <v>212</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D55" s="5">
         <v>1</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="5" t="s">
-        <v>203</v>
+        <v>213</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>212</v>
+        <v>54</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>213</v>
+        <v>231</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>214</v>
+        <v>230</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>215</v>
+        <v>229</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D56" s="5">
         <v>1</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="5" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>54</v>
+        <v>205</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>234</v>
+        <v>206</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>233</v>
+        <v>207</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>232</v>
+        <v>208</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>52</v>
+        <v>78</v>
       </c>
       <c r="D57" s="5">
         <v>1</v>
       </c>
       <c r="E57" s="5"/>
       <c r="F57" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="I57" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="G57" s="5" t="s">
-        <v>208</v>
-      </c>
-      <c r="H57" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="I57" s="5" t="s">
-        <v>210</v>
-      </c>
       <c r="J57" s="5" t="s">
-        <v>211</v>
+        <v>204</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="D58" s="5">
         <v>1</v>
       </c>
       <c r="E58" s="5"/>
       <c r="F58" s="5" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>205</v>
+        <v>198</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>88</v>
+        <v>233</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D59" s="5">
         <v>1</v>
       </c>
       <c r="E59" s="5"/>
       <c r="F59" s="5" t="s">
-        <v>198</v>
+        <v>164</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>199</v>
+        <v>235</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>201</v>
+        <v>236</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>200</v>
+        <v>237</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>202</v>
+        <v>238</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>80</v>
+        <v>147</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>236</v>
+        <v>22</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>81</v>
+        <v>23</v>
       </c>
       <c r="D60" s="5">
-        <v>1</v>
-      </c>
-      <c r="E60" s="5"/>
-      <c r="F60" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="G60" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="H60" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="I60" s="5" t="s">
-        <v>240</v>
-      </c>
-      <c r="J60" s="5" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="B61" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D61" s="5">
         <v>2</v>
       </c>
-      <c r="E61" s="5" t="s">
-        <v>130</v>
-      </c>
-      <c r="F61" s="5"/>
-      <c r="G61" s="5"/>
-      <c r="H61" s="5"/>
-      <c r="I61" s="5"/>
-      <c r="J61" s="5"/>
+      <c r="E60" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F60" s="5"/>
+      <c r="G60" s="5"/>
+      <c r="H60" s="5"/>
+      <c r="I60" s="5"/>
+      <c r="J60" s="5"/>
     </row>
   </sheetData>
   <sortState ref="A9:J60">

</xml_diff>

<commit_message>
add fuses for connectable headers (adc, encoder, motors, servo, codec). GERBER/BOM UPDATES ONLY
</commit_message>
<xml_diff>
--- a/pcb/labio.bom.xlsx
+++ b/pcb/labio.bom.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="249">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="267">
   <si>
     <t>Source</t>
   </si>
@@ -774,6 +774,60 @@
   </si>
   <si>
     <t>R303, R304, R601, R602</t>
+  </si>
+  <si>
+    <t>F601</t>
+  </si>
+  <si>
+    <t>F_Small</t>
+  </si>
+  <si>
+    <t>F602</t>
+  </si>
+  <si>
+    <t>F301, F603, F701</t>
+  </si>
+  <si>
+    <t>Littelfuse</t>
+  </si>
+  <si>
+    <t>0154004.DRT</t>
+  </si>
+  <si>
+    <t>FUSE BRD MNT 4A 125VAC/VDC 2SMD</t>
+  </si>
+  <si>
+    <t>F1309CT-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/littelfuse-inc/0154004.DRT/F1309CT-ND/266657</t>
+  </si>
+  <si>
+    <t>PTC RESTTBLE 0.10A 60V CHIP 1206</t>
+  </si>
+  <si>
+    <t>507-1794-1-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/bel-fuse-inc/0ZCJ0010FF2E/507-1794-1-ND/4156222</t>
+  </si>
+  <si>
+    <t>0ZCJ0010FF2E</t>
+  </si>
+  <si>
+    <t>Bel Fuse</t>
+  </si>
+  <si>
+    <t>0ZCJ0050AF2E</t>
+  </si>
+  <si>
+    <t>PTC RESTTBLE 0.50A 24V CHIP 1206</t>
+  </si>
+  <si>
+    <t>507-1803-1-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/bel-fuse-inc/0ZCJ0050AF2E/507-1803-1-ND/4156312</t>
   </si>
 </sst>
 </file>
@@ -1123,11 +1177,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J60"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1474,79 +1528,101 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>111</v>
+        <v>252</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>113</v>
+        <v>71</v>
       </c>
       <c r="D19" s="5">
-        <v>1</v>
-      </c>
-      <c r="E19" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>260</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>106</v>
+        <v>249</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>107</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>108</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="C20" s="5"/>
       <c r="D20" s="5">
         <v>1</v>
       </c>
-      <c r="E20" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="5"/>
-      <c r="J20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>114</v>
+        <v>251</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>112</v>
+        <v>250</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>115</v>
+        <v>71</v>
       </c>
       <c r="D21" s="5">
         <v>1</v>
       </c>
-      <c r="E21" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>266</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="D22" s="5">
         <v>1</v>
@@ -1560,37 +1636,37 @@
       <c r="I22" s="5"/>
       <c r="J22" s="5"/>
     </row>
-    <row r="23" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>131</v>
+        <v>106</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D23" s="5">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E23" s="5" t="s">
         <v>129</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
+      <c r="H23" s="6"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>16</v>
+        <v>114</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>17</v>
+        <v>112</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>18</v>
+        <v>115</v>
       </c>
       <c r="D24" s="5">
         <v>1</v>
@@ -1606,48 +1682,42 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>83</v>
+        <v>109</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>84</v>
+        <v>107</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>85</v>
+        <v>110</v>
       </c>
       <c r="D25" s="5">
         <v>1</v>
       </c>
-      <c r="E25" s="5"/>
-      <c r="F25" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="G25" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="H25" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E25" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="5"/>
+      <c r="J25" s="5"/>
+    </row>
+    <row r="26" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>13</v>
+        <v>131</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>14</v>
+        <v>104</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>15</v>
+        <v>105</v>
       </c>
       <c r="D26" s="5">
-        <v>1</v>
-      </c>
-      <c r="E26" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>129</v>
+      </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
       <c r="H26" s="5"/>
@@ -1656,16 +1726,16 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>135</v>
+        <v>16</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="D27" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>129</v>
@@ -1678,50 +1748,48 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>45</v>
+        <v>83</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>47</v>
+        <v>85</v>
       </c>
       <c r="D28" s="5">
         <v>1</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="H28" s="5" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="I28" s="5" t="s">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>189</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>133</v>
+        <v>13</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>65</v>
+        <v>14</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>66</v>
+        <v>15</v>
       </c>
       <c r="D29" s="5">
         <v>1</v>
       </c>
-      <c r="E29" s="5" t="s">
-        <v>129</v>
-      </c>
+      <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
@@ -1730,16 +1798,16 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>62</v>
+        <v>34</v>
       </c>
       <c r="D30" s="5">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>129</v>
@@ -1752,35 +1820,43 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>136</v>
+        <v>45</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D31" s="5">
-        <v>2</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>189</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>81</v>
+        <v>133</v>
       </c>
       <c r="B32" s="5" t="s">
         <v>65</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="D32" s="5">
         <v>1</v>
@@ -1796,16 +1872,16 @@
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>101</v>
+        <v>134</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>102</v>
+        <v>61</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="D33" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E33" s="5" t="s">
         <v>129</v>
@@ -1818,78 +1894,64 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>35</v>
+        <v>136</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>37</v>
+        <v>64</v>
       </c>
       <c r="D34" s="5">
-        <v>1</v>
-      </c>
-      <c r="E34" s="5"/>
-      <c r="F34" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="G34" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="I34" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="J34" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5"/>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5"/>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>142</v>
+        <v>81</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="D35" s="5">
-        <v>15</v>
-      </c>
-      <c r="E35" s="5"/>
-      <c r="F35" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="G35" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="I35" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="J35" s="5" t="s">
-        <v>218</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E35" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>24</v>
+        <v>102</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="D36" s="5">
-        <v>2</v>
-      </c>
-      <c r="E36" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="E36" s="5" t="s">
+        <v>129</v>
+      </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
       <c r="H36" s="5"/>
@@ -1898,58 +1960,76 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>143</v>
+        <v>36</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D37" s="5">
         <v>1</v>
       </c>
-      <c r="E37" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E37" s="5"/>
+      <c r="F37" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>144</v>
+        <v>43</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="D38" s="5">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E38" s="5"/>
-      <c r="F38" s="5"/>
-      <c r="G38" s="5"/>
-      <c r="H38" s="5"/>
-      <c r="I38" s="5"/>
-      <c r="J38" s="5"/>
+      <c r="F38" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>38</v>
+        <v>146</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="C39" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D39" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
@@ -1958,20 +2038,22 @@
       <c r="I39" s="5"/>
       <c r="J39" s="5"/>
     </row>
-    <row r="40" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B40" s="5">
-        <v>220</v>
+        <v>19</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>143</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D40" s="5">
-        <v>19</v>
-      </c>
-      <c r="E40" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>129</v>
+      </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
@@ -1980,16 +2062,16 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>248</v>
+        <v>145</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>20</v>
+        <v>144</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D41" s="5">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
@@ -1998,18 +2080,18 @@
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B42" s="5">
-        <v>0</v>
+        <v>38</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D42" s="5">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
@@ -2018,40 +2100,38 @@
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>56</v>
+        <v>139</v>
+      </c>
+      <c r="B43" s="5">
+        <v>220</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D43" s="5">
-        <v>3</v>
-      </c>
-      <c r="E43" s="5" t="s">
-        <v>129</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E43" s="5"/>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
       <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>138</v>
+        <v>248</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>72</v>
+        <v>20</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D44" s="5">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
@@ -2060,18 +2140,18 @@
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="B45" s="5">
-        <v>0.01</v>
+        <v>0</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="D45" s="5">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
@@ -2082,36 +2162,38 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>94</v>
+        <v>140</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>95</v>
+        <v>56</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D46" s="5">
-        <v>1</v>
-      </c>
-      <c r="E46" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>129</v>
+      </c>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>96</v>
+        <v>138</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>97</v>
+        <v>72</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D47" s="5">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
@@ -2120,287 +2202,257 @@
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>40</v>
+        <v>141</v>
+      </c>
+      <c r="B48" s="5">
+        <v>0.01</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="D48" s="5">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="E48" s="5"/>
-      <c r="F48" s="5" t="s">
-        <v>180</v>
-      </c>
-      <c r="G48" s="5" t="s">
-        <v>181</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="I48" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="J48" s="5" t="s">
-        <v>184</v>
-      </c>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5"/>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>73</v>
+        <v>94</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>74</v>
+        <v>95</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>75</v>
+        <v>21</v>
       </c>
       <c r="D49" s="5">
         <v>1</v>
       </c>
-      <c r="E49" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F49" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="G49" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="I49" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="J49" s="5" t="s">
-        <v>247</v>
-      </c>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5"/>
+      <c r="I49" s="5"/>
+      <c r="J49" s="5"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>99</v>
+        <v>21</v>
       </c>
       <c r="D50" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E50" s="5"/>
-      <c r="F50" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>162</v>
-      </c>
-      <c r="J50" s="5" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+    </row>
+    <row r="51" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>25</v>
+        <v>130</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="D51" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E51" s="5"/>
       <c r="F51" s="5" t="s">
-        <v>148</v>
+        <v>180</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>149</v>
+        <v>181</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>153</v>
+        <v>182</v>
       </c>
       <c r="I51" s="5" t="s">
-        <v>150</v>
+        <v>183</v>
       </c>
       <c r="J51" s="5" t="s">
-        <v>151</v>
+        <v>184</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>31</v>
+        <v>74</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="D52" s="5">
         <v>1</v>
       </c>
-      <c r="E52" s="5"/>
+      <c r="E52" s="5" t="s">
+        <v>129</v>
+      </c>
       <c r="F52" s="5" t="s">
-        <v>165</v>
+        <v>243</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>166</v>
+        <v>244</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>168</v>
+        <v>245</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>167</v>
+        <v>246</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>169</v>
+        <v>247</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>234</v>
+        <v>121</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C53" s="5"/>
+        <v>98</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>99</v>
+      </c>
       <c r="D53" s="5">
-        <v>1</v>
-      </c>
-      <c r="E53" s="5" t="s">
-        <v>129</v>
-      </c>
+        <v>5</v>
+      </c>
+      <c r="E53" s="5"/>
       <c r="F53" s="5" t="s">
-        <v>240</v>
+        <v>159</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>239</v>
+        <v>160</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>241</v>
+        <v>161</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>230</v>
+        <v>162</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>242</v>
+        <v>163</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>51</v>
+        <v>26</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="D54" s="5">
         <v>1</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="5" t="s">
-        <v>200</v>
+        <v>148</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>209</v>
+        <v>149</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>210</v>
+        <v>153</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>211</v>
+        <v>150</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>212</v>
+        <v>151</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>53</v>
+        <v>30</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>54</v>
+        <v>31</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="D55" s="5">
         <v>1</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="5" t="s">
-        <v>213</v>
+        <v>165</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>54</v>
+        <v>166</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>231</v>
+        <v>168</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>230</v>
+        <v>167</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>229</v>
+        <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>59</v>
+        <v>234</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>52</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="C56" s="5"/>
       <c r="D56" s="5">
         <v>1</v>
       </c>
-      <c r="E56" s="5"/>
+      <c r="E56" s="5" t="s">
+        <v>129</v>
+      </c>
       <c r="F56" s="5" t="s">
-        <v>200</v>
+        <v>240</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>205</v>
+        <v>239</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>206</v>
+        <v>241</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>207</v>
+        <v>230</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>208</v>
+        <v>242</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="D57" s="5">
         <v>1</v>
@@ -2410,99 +2462,189 @@
         <v>200</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>201</v>
+        <v>209</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>202</v>
+        <v>210</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>203</v>
+        <v>211</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>204</v>
+        <v>212</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>86</v>
+        <v>53</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>87</v>
+        <v>54</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>88</v>
+        <v>55</v>
       </c>
       <c r="D58" s="5">
         <v>1</v>
       </c>
       <c r="E58" s="5"/>
       <c r="F58" s="5" t="s">
-        <v>195</v>
+        <v>213</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>196</v>
+        <v>54</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>198</v>
+        <v>231</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>197</v>
+        <v>230</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>199</v>
+        <v>229</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>233</v>
+        <v>60</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="D59" s="5">
         <v>1</v>
       </c>
       <c r="E59" s="5"/>
       <c r="F59" s="5" t="s">
-        <v>164</v>
+        <v>200</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>235</v>
+        <v>205</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>236</v>
+        <v>206</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>237</v>
+        <v>207</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>238</v>
+        <v>208</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D60" s="5">
+        <v>1</v>
+      </c>
+      <c r="E60" s="5"/>
+      <c r="F60" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="H60" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="I60" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="J60" s="5" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="D61" s="5">
+        <v>1</v>
+      </c>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="H61" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="I61" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="J61" s="5" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D62" s="5">
+        <v>1</v>
+      </c>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="H62" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="I62" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="J62" s="5" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="B63" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C63" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D60" s="5">
+      <c r="D63" s="5">
         <v>2</v>
       </c>
-      <c r="E60" s="5" t="s">
+      <c r="E63" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="F60" s="5"/>
-      <c r="G60" s="5"/>
-      <c r="H60" s="5"/>
-      <c r="I60" s="5"/>
-      <c r="J60" s="5"/>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
     </row>
   </sheetData>
   <sortState ref="A9:J60">

</xml_diff>

<commit_message>
fix codec/mic/trrs bias circuit
* trrs (headset) mic bias was flipped (in vs out) from datasheet
* trrs l/r decoupling caps changed back to 220uF per datasheet and re-layout for 1210 ceramic
* mems mic decoupling changed to 1uF for consistency
</commit_message>
<xml_diff>
--- a/pcb/labio.bom.xlsx
+++ b/pcb/labio.bom.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="317" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="274">
   <si>
     <t>Source</t>
   </si>
@@ -398,9 +398,6 @@
     <t>C201, C202, C301, C502, C503, C504, C506, C510, C511, C601, C602, C605, C606, C607, C701, C703, C705, C707, C708, C710, C713, C717</t>
   </si>
   <si>
-    <t>C709, C714, C715</t>
-  </si>
-  <si>
     <t>C801, C802, C803, C804, C805</t>
   </si>
   <si>
@@ -828,6 +825,30 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/bel-fuse-inc/0ZCJ0050AF2E/507-1803-1-ND/4156312</t>
+  </si>
+  <si>
+    <t>C714, C715</t>
+  </si>
+  <si>
+    <t>220uF</t>
+  </si>
+  <si>
+    <t>C709</t>
+  </si>
+  <si>
+    <t>CL32A227MQVNNNE</t>
+  </si>
+  <si>
+    <t>220µF 6.3V Ceramic Capacitor X5R 1210</t>
+  </si>
+  <si>
+    <t>1276-3375-1-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/CL32A227MQVNNNE/1276-3375-1-ND/3891461</t>
+  </si>
+  <si>
+    <t>Capacitors_SMD:C_1210</t>
   </si>
 </sst>
 </file>
@@ -1177,11 +1198,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I21" sqref="I21"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1217,7 +1238,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1266,7 +1287,7 @@
         <v>116</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>117</v>
@@ -1275,7 +1296,7 @@
         <v>118</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>119</v>
@@ -1306,7 +1327,7 @@
     </row>
     <row r="10" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>48</v>
@@ -1319,19 +1340,19 @@
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>224</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="H10" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="I10" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>227</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
@@ -1356,7 +1377,7 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>67</v>
@@ -1369,19 +1390,19 @@
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="G12" s="5" t="s">
         <v>219</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="H12" s="5" t="s">
         <v>220</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="I12" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="J12" s="5" t="s">
         <v>222</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
@@ -1406,7 +1427,7 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>123</v>
+        <v>268</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>91</v>
@@ -1415,7 +1436,7 @@
         <v>29</v>
       </c>
       <c r="D14" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -1446,255 +1467,263 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>124</v>
+        <v>266</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>273</v>
+      </c>
+      <c r="D16" s="5">
+        <v>2</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>271</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C17" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D16" s="5">
+      <c r="D17" s="5">
         <v>5</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B17" s="5" t="s">
+      <c r="E17" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D18" s="5">
         <v>19</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="G17" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="H17" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="I17" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="5">
-        <v>12</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5" t="s">
-        <v>154</v>
+        <v>189</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>155</v>
+        <v>190</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>156</v>
+        <v>191</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>157</v>
+        <v>192</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>252</v>
+        <v>126</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>250</v>
+        <v>69</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D19" s="5">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5" t="s">
-        <v>262</v>
+        <v>153</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>261</v>
+        <v>154</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>258</v>
+        <v>155</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>259</v>
+        <v>156</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>260</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B20" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="B20" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="C20" s="5"/>
+      <c r="C20" s="5" t="s">
+        <v>71</v>
+      </c>
       <c r="D20" s="5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5" t="s">
-        <v>253</v>
+        <v>261</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>254</v>
+        <v>260</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>71</v>
-      </c>
+        <v>249</v>
+      </c>
+      <c r="C21" s="5"/>
       <c r="D21" s="5">
         <v>1</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>111</v>
+        <v>250</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>112</v>
+        <v>249</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>113</v>
+        <v>71</v>
       </c>
       <c r="D22" s="5">
         <v>1</v>
       </c>
-      <c r="E22" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5" t="s">
+        <v>261</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>265</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="D23" s="5">
         <v>1</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="6"/>
+      <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D24" s="5">
         <v>1</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+      <c r="H24" s="6"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="D25" s="5">
         <v>1</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -1702,21 +1731,21 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="D26" s="5">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
@@ -1724,21 +1753,21 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>16</v>
+        <v>130</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>17</v>
+        <v>104</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>18</v>
+        <v>105</v>
       </c>
       <c r="D27" s="5">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -1748,70 +1777,70 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>83</v>
+        <v>16</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>84</v>
+        <v>17</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>85</v>
+        <v>18</v>
       </c>
       <c r="D28" s="5">
         <v>1</v>
       </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>179</v>
-      </c>
+      <c r="E28" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>13</v>
+        <v>83</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>14</v>
+        <v>84</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>15</v>
+        <v>85</v>
       </c>
       <c r="D29" s="5">
         <v>1</v>
       </c>
       <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
+      <c r="F29" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>135</v>
+        <v>13</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>34</v>
+        <v>15</v>
       </c>
       <c r="D30" s="5">
-        <v>7</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>129</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
@@ -1820,71 +1849,71 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>45</v>
+        <v>134</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D31" s="5">
-        <v>1</v>
-      </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>188</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>189</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>133</v>
+        <v>45</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>65</v>
+        <v>46</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="D32" s="5">
         <v>1</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>188</v>
+      </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="D33" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
@@ -1894,19 +1923,19 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D34" s="5">
         <v>2</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
@@ -1916,19 +1945,19 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>81</v>
+        <v>135</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="D35" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
@@ -1938,19 +1967,19 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>102</v>
+        <v>65</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="D36" s="5">
         <v>1</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
@@ -1960,100 +1989,100 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="5">
+        <v>1</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="B38" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="5" t="s">
+      <c r="C38" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="D37" s="5">
-        <v>1</v>
-      </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="G37" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="H37" s="5" t="s">
-        <v>172</v>
-      </c>
-      <c r="I37" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="J37" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="C38" s="5" t="s">
-        <v>44</v>
-      </c>
       <c r="D38" s="5">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="I38" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D39" s="5">
+        <v>15</v>
+      </c>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="G39" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="H39" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="I39" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="I38" s="5" t="s">
+      <c r="J39" s="5" t="s">
         <v>217</v>
       </c>
-      <c r="J38" s="5" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D39" s="5">
-        <v>2</v>
-      </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>19</v>
+        <v>145</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>143</v>
+        <v>24</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D40" s="5">
-        <v>1</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>129</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
@@ -2062,18 +2091,20 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>145</v>
+        <v>19</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D41" s="5">
-        <v>2</v>
-      </c>
-      <c r="E41" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>128</v>
+      </c>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
@@ -2082,16 +2113,16 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>38</v>
+        <v>144</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>39</v>
+        <v>143</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D42" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
@@ -2100,18 +2131,18 @@
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B43" s="5">
-        <v>220</v>
+        <v>38</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>39</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D43" s="5">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
@@ -2120,18 +2151,18 @@
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>248</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>20</v>
+        <v>138</v>
+      </c>
+      <c r="B44" s="5">
+        <v>220</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D44" s="5">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
@@ -2140,18 +2171,18 @@
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>137</v>
-      </c>
-      <c r="B45" s="5">
-        <v>0</v>
+        <v>247</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>20</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D45" s="5">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="E45" s="5"/>
       <c r="F45" s="5"/>
@@ -2160,60 +2191,60 @@
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>56</v>
+        <v>136</v>
+      </c>
+      <c r="B46" s="5">
+        <v>0</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D46" s="5">
-        <v>3</v>
-      </c>
-      <c r="E46" s="5" t="s">
-        <v>129</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="E46" s="5"/>
       <c r="F46" s="5"/>
       <c r="G46" s="5"/>
       <c r="H46" s="5"/>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>72</v>
+        <v>56</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D47" s="5">
-        <v>15</v>
-      </c>
-      <c r="E47" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>128</v>
+      </c>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>141</v>
-      </c>
-      <c r="B48" s="5">
-        <v>0.01</v>
+        <v>137</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="D48" s="5">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
@@ -2224,16 +2255,16 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B49" s="5" t="s">
-        <v>95</v>
+        <v>140</v>
+      </c>
+      <c r="B49" s="5">
+        <v>0.01</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>21</v>
+        <v>71</v>
       </c>
       <c r="D49" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -2244,10 +2275,10 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C50" s="5" t="s">
         <v>21</v>
@@ -2262,389 +2293,409 @@
       <c r="I50" s="5"/>
       <c r="J50" s="5"/>
     </row>
-    <row r="51" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>130</v>
+        <v>96</v>
       </c>
       <c r="B51" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D51" s="5">
+        <v>1</v>
+      </c>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="5"/>
+      <c r="H51" s="5"/>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
+    </row>
+    <row r="52" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A52" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="C52" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D51" s="5">
+      <c r="D52" s="5">
         <v>10</v>
       </c>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5" t="s">
+      <c r="E52" s="5"/>
+      <c r="F52" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="G52" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="G51" s="5" t="s">
+      <c r="H52" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="H51" s="5" t="s">
+      <c r="I52" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="I51" s="5" t="s">
+      <c r="J52" s="5" t="s">
         <v>183</v>
-      </c>
-      <c r="J51" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A52" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B52" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="C52" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="D52" s="5">
-        <v>1</v>
-      </c>
-      <c r="E52" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>243</v>
-      </c>
-      <c r="G52" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>121</v>
+        <v>73</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="D53" s="5">
-        <v>5</v>
-      </c>
-      <c r="E53" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>128</v>
+      </c>
       <c r="F53" s="5" t="s">
-        <v>159</v>
+        <v>242</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>160</v>
+        <v>243</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>161</v>
+        <v>244</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>162</v>
+        <v>245</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>163</v>
+        <v>246</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>25</v>
+        <v>121</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>26</v>
+        <v>98</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>27</v>
+        <v>99</v>
       </c>
       <c r="D54" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="5" t="s">
-        <v>148</v>
+        <v>158</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>149</v>
+        <v>159</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>151</v>
+        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="D55" s="5">
         <v>1</v>
       </c>
       <c r="E55" s="5"/>
       <c r="F55" s="5" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>168</v>
+        <v>152</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>169</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>234</v>
+        <v>30</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C56" s="5"/>
+        <v>31</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="D56" s="5">
         <v>1</v>
       </c>
-      <c r="E56" s="5" t="s">
-        <v>129</v>
-      </c>
+      <c r="E56" s="5"/>
       <c r="F56" s="5" t="s">
-        <v>240</v>
+        <v>164</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>239</v>
+        <v>165</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>241</v>
+        <v>167</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>230</v>
+        <v>166</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>242</v>
+        <v>168</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>50</v>
+        <v>233</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>52</v>
-      </c>
+        <v>238</v>
+      </c>
+      <c r="C57" s="5"/>
       <c r="D57" s="5">
         <v>1</v>
       </c>
-      <c r="E57" s="5"/>
+      <c r="E57" s="5" t="s">
+        <v>128</v>
+      </c>
       <c r="F57" s="5" t="s">
-        <v>200</v>
+        <v>239</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>209</v>
+        <v>238</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>210</v>
+        <v>240</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>212</v>
+        <v>241</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D58" s="5">
         <v>1</v>
       </c>
       <c r="E58" s="5"/>
       <c r="F58" s="5" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>54</v>
+        <v>208</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>231</v>
+        <v>209</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>230</v>
+        <v>210</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>229</v>
+        <v>211</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="D59" s="5">
         <v>1</v>
       </c>
       <c r="E59" s="5"/>
       <c r="F59" s="5" t="s">
-        <v>200</v>
+        <v>212</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>205</v>
+        <v>54</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>206</v>
+        <v>230</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>207</v>
+        <v>229</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>208</v>
+        <v>228</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>76</v>
+        <v>59</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>77</v>
+        <v>60</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
       <c r="D60" s="5">
         <v>1</v>
       </c>
       <c r="E60" s="5"/>
       <c r="F60" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="D61" s="5">
         <v>1</v>
       </c>
       <c r="E61" s="5"/>
       <c r="F61" s="5" t="s">
-        <v>195</v>
+        <v>199</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>197</v>
+        <v>202</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>233</v>
+        <v>87</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="D62" s="5">
         <v>1</v>
       </c>
       <c r="E62" s="5"/>
       <c r="F62" s="5" t="s">
-        <v>164</v>
+        <v>194</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>235</v>
+        <v>195</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>236</v>
+        <v>197</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>237</v>
+        <v>196</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>238</v>
+        <v>198</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>147</v>
+        <v>79</v>
       </c>
       <c r="B63" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D63" s="5">
+        <v>1</v>
+      </c>
+      <c r="E63" s="5"/>
+      <c r="F63" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="B64" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C63" s="5" t="s">
+      <c r="C64" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D63" s="5">
+      <c r="D64" s="5">
         <v>2</v>
       </c>
-      <c r="E63" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
-      <c r="J63" s="5"/>
+      <c r="E64" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
     </row>
   </sheetData>
   <sortState ref="A9:J60">

</xml_diff>

<commit_message>
Fix i2c addresses, pressure sensor footprint, consolidate BOM
* Schematic should list I2C addresses for accelerometer, gyro.
* Pressure sensor footprint (U502) has pins in the wrong order. Redraw footprint and adjust routing.
* Bump i2c and photodiode pullups to 2.2k
* Remove R505 near gyro
</commit_message>
<xml_diff>
--- a/pcb/labio.bom.xlsx
+++ b/pcb/labio.bom.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="276">
   <si>
     <t>Source</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Measurement_Points:Measurement_Point_Round-SMD-Pad_Small</t>
   </si>
   <si>
-    <t>4.7k</t>
-  </si>
-  <si>
     <t>U201</t>
   </si>
   <si>
@@ -143,12 +140,6 @@
     <t>LEDs:LED-0603</t>
   </si>
   <si>
-    <t>R301</t>
-  </si>
-  <si>
-    <t>1.5k</t>
-  </si>
-  <si>
     <t>DIP_SWITCH_X04</t>
   </si>
   <si>
@@ -296,18 +287,9 @@
     <t>labio-special:SPU0410HR5H</t>
   </si>
   <si>
-    <t>C704</t>
-  </si>
-  <si>
-    <t>2.2uF</t>
-  </si>
-  <si>
     <t>220pF</t>
   </si>
   <si>
-    <t>C711</t>
-  </si>
-  <si>
     <t>1uF</t>
   </si>
   <si>
@@ -317,9 +299,6 @@
     <t>47k</t>
   </si>
   <si>
-    <t>R703</t>
-  </si>
-  <si>
     <t>2.2k</t>
   </si>
   <si>
@@ -437,9 +416,6 @@
     <t>P607, P608</t>
   </si>
   <si>
-    <t>R401, R402, R403, R502, R504, R505, R506, R507, R508, R509, R510, R511, R513, R515</t>
-  </si>
-  <si>
     <t>R603, R604, R608, R609, R610, R611, R616, R617, R620, R621, R625, R628, R629, R632, R633</t>
   </si>
   <si>
@@ -464,9 +440,6 @@
     <t>R204, R205</t>
   </si>
   <si>
-    <t>R201, R202</t>
-  </si>
-  <si>
     <t>W201, W202</t>
   </si>
   <si>
@@ -770,9 +743,6 @@
     <t>http://www.digikey.com/product-detail/en/bourns-inc/PEC12R-4220F-N0024/PEC12R-4220F-N0024-ND/4499652</t>
   </si>
   <si>
-    <t>R303, R304, R601, R602</t>
-  </si>
-  <si>
     <t>F601</t>
   </si>
   <si>
@@ -782,9 +752,6 @@
     <t>F602</t>
   </si>
   <si>
-    <t>F301, F603, F701</t>
-  </si>
-  <si>
     <t>Littelfuse</t>
   </si>
   <si>
@@ -849,6 +816,45 @@
   </si>
   <si>
     <t>Capacitors_SMD:C_1210</t>
+  </si>
+  <si>
+    <t>F301, F401, F501, F603, F604, F701</t>
+  </si>
+  <si>
+    <t>U703</t>
+  </si>
+  <si>
+    <t>OPA344_SOT23-5</t>
+  </si>
+  <si>
+    <t>OPA344NA/250</t>
+  </si>
+  <si>
+    <t>IC OPAMP GP 1MHZ RRO SOT23-5</t>
+  </si>
+  <si>
+    <t>OPA344NACT-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/texas-instruments/OPA344NA-250/OPA344NACT-ND/362263</t>
+  </si>
+  <si>
+    <t>C711, C704,  C719, C720</t>
+  </si>
+  <si>
+    <t>R303, R304, R601, R602, R704, R705, R706</t>
+  </si>
+  <si>
+    <t>R707</t>
+  </si>
+  <si>
+    <t>820k</t>
+  </si>
+  <si>
+    <t>R201, R202, R301, R703</t>
+  </si>
+  <si>
+    <t>R401, R402, R403, R502, R504, R506, R507, R508, R509, R510, R511, R513, R515</t>
   </si>
 </sst>
 </file>
@@ -1198,11 +1204,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <pane ySplit="8" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1238,7 +1244,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1284,36 +1290,36 @@
         <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>28</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>29</v>
       </c>
       <c r="D9" s="5">
         <v>22</v>
@@ -1327,43 +1333,43 @@
     </row>
     <row r="10" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D10" s="5">
         <v>10</v>
       </c>
       <c r="E10" s="5"/>
       <c r="F10" s="5" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="H10" s="5" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="I10" s="5" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="J10" s="5" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D11" s="5">
         <v>1</v>
@@ -1377,43 +1383,43 @@
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D12" s="5">
         <v>4</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="5" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="I12" s="5" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="J12" s="5" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>89</v>
+        <v>257</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D13" s="5">
         <v>1</v>
@@ -1427,16 +1433,16 @@
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D14" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
@@ -1447,252 +1453,254 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>92</v>
+        <v>255</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>93</v>
+        <v>256</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>29</v>
+        <v>262</v>
       </c>
       <c r="D15" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
+      <c r="F15" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>260</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>266</v>
+        <v>116</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>267</v>
+        <v>93</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>273</v>
+        <v>28</v>
       </c>
       <c r="D16" s="5">
-        <v>2</v>
-      </c>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5" t="s">
-        <v>223</v>
-      </c>
-      <c r="G16" s="5" t="s">
-        <v>269</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>270</v>
-      </c>
-      <c r="I16" s="5" t="s">
-        <v>271</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>100</v>
+        <v>39</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="D17" s="5">
-        <v>5</v>
-      </c>
-      <c r="E17" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>37</v>
+        <v>67</v>
       </c>
       <c r="D18" s="5">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5" t="s">
-        <v>189</v>
+        <v>144</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>190</v>
+        <v>145</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>191</v>
+        <v>146</v>
       </c>
       <c r="I18" s="5" t="s">
-        <v>192</v>
+        <v>147</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>126</v>
+        <v>263</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>69</v>
+        <v>239</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D19" s="5">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5" t="s">
-        <v>153</v>
+        <v>250</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>154</v>
+        <v>249</v>
       </c>
       <c r="H19" s="5" t="s">
-        <v>155</v>
+        <v>246</v>
       </c>
       <c r="I19" s="5" t="s">
-        <v>156</v>
+        <v>247</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>157</v>
+        <v>248</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>71</v>
-      </c>
+        <v>239</v>
+      </c>
+      <c r="C20" s="5"/>
       <c r="D20" s="5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5" t="s">
-        <v>261</v>
+        <v>241</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>260</v>
+        <v>242</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>258</v>
+        <v>244</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>259</v>
+        <v>245</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="C21" s="5"/>
+        <v>239</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>68</v>
+      </c>
       <c r="D21" s="5">
         <v>1</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="H21" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="G21" s="5" t="s">
+      <c r="I21" s="5" t="s">
         <v>253</v>
       </c>
-      <c r="H21" s="5" t="s">
+      <c r="J21" s="5" t="s">
         <v>254</v>
-      </c>
-      <c r="I21" s="5" t="s">
-        <v>255</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>256</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>250</v>
+        <v>104</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>249</v>
+        <v>105</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>71</v>
+        <v>106</v>
       </c>
       <c r="D22" s="5">
         <v>1</v>
       </c>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5" t="s">
-        <v>261</v>
-      </c>
-      <c r="G22" s="5" t="s">
-        <v>262</v>
-      </c>
-      <c r="H22" s="5" t="s">
-        <v>263</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>265</v>
-      </c>
+      <c r="E22" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
       <c r="D23" s="5">
         <v>1</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
+      <c r="H23" s="6"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>108</v>
@@ -1701,29 +1709,29 @@
         <v>1</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="6"/>
+      <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
       <c r="D25" s="5">
         <v>1</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -1731,21 +1739,21 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>109</v>
+        <v>123</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
       <c r="D26" s="5">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
@@ -1753,21 +1761,21 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>130</v>
+        <v>16</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>104</v>
+        <v>17</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>105</v>
+        <v>18</v>
       </c>
       <c r="D27" s="5">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -1777,70 +1785,70 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>16</v>
+        <v>80</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>17</v>
+        <v>81</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>18</v>
+        <v>82</v>
       </c>
       <c r="D28" s="5">
         <v>1</v>
       </c>
-      <c r="E28" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="5"/>
-      <c r="J28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="G28" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="H28" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="I28" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>169</v>
+      </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>83</v>
+        <v>13</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>84</v>
+        <v>14</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>85</v>
+        <v>15</v>
       </c>
       <c r="D29" s="5">
         <v>1</v>
       </c>
       <c r="E29" s="5"/>
-      <c r="F29" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>178</v>
-      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>13</v>
+        <v>127</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>15</v>
+        <v>33</v>
       </c>
       <c r="D30" s="5">
-        <v>1</v>
-      </c>
-      <c r="E30" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>121</v>
+      </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
       <c r="H30" s="5"/>
@@ -1849,71 +1857,71 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>134</v>
+        <v>42</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>33</v>
+        <v>43</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="D31" s="5">
-        <v>7</v>
-      </c>
-      <c r="E31" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F31" s="5"/>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="I31" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>45</v>
+        <v>125</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>46</v>
+        <v>62</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="D32" s="5">
         <v>1</v>
       </c>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>185</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>186</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="J32" s="5" t="s">
-        <v>188</v>
-      </c>
+      <c r="E32" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>65</v>
+        <v>58</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
       <c r="D33" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
@@ -1923,19 +1931,19 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B34" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="D34" s="5">
         <v>2</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
@@ -1945,19 +1953,19 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>135</v>
+        <v>78</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="D35" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
@@ -1967,19 +1975,19 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>81</v>
+        <v>94</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>65</v>
+        <v>95</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="D36" s="5">
         <v>1</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
@@ -1989,100 +1997,100 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>101</v>
+        <v>34</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>102</v>
+        <v>35</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>103</v>
+        <v>36</v>
       </c>
       <c r="D37" s="5">
         <v>1</v>
       </c>
-      <c r="E37" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F37" s="5"/>
-      <c r="G37" s="5"/>
-      <c r="H37" s="5"/>
-      <c r="I37" s="5"/>
-      <c r="J37" s="5"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="E37" s="5"/>
+      <c r="F37" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="I37" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>35</v>
+        <v>133</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C38" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="D38" s="5">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5" t="s">
-        <v>169</v>
+        <v>204</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>170</v>
+        <v>205</v>
       </c>
       <c r="H38" s="5" t="s">
-        <v>171</v>
+        <v>206</v>
       </c>
       <c r="I38" s="5" t="s">
-        <v>172</v>
+        <v>207</v>
       </c>
       <c r="J38" s="5" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>141</v>
+        <v>274</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>43</v>
+        <v>90</v>
       </c>
       <c r="C39" s="5" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="D39" s="5">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E39" s="5"/>
-      <c r="F39" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="G39" s="5" t="s">
-        <v>214</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>215</v>
-      </c>
-      <c r="I39" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>217</v>
-      </c>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>145</v>
+        <v>19</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>24</v>
+        <v>134</v>
       </c>
       <c r="C40" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D40" s="5">
-        <v>2</v>
-      </c>
-      <c r="E40" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="E40" s="5" t="s">
+        <v>121</v>
+      </c>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
       <c r="H40" s="5"/>
@@ -2091,38 +2099,36 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>19</v>
+        <v>136</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D41" s="5">
-        <v>1</v>
-      </c>
-      <c r="E41" s="5" t="s">
-        <v>128</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>143</v>
+        <v>130</v>
+      </c>
+      <c r="B42" s="5">
+        <v>220</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D42" s="5">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
@@ -2133,16 +2139,16 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>38</v>
+        <v>271</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D43" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E43" s="5"/>
       <c r="F43" s="5"/>
@@ -2151,18 +2157,18 @@
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>138</v>
+        <v>275</v>
       </c>
       <c r="B44" s="5">
-        <v>220</v>
+        <v>0</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D44" s="5">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E44" s="5"/>
       <c r="F44" s="5"/>
@@ -2173,18 +2179,20 @@
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>247</v>
+        <v>131</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>20</v>
+        <v>53</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D45" s="5">
-        <v>4</v>
-      </c>
-      <c r="E45" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="E45" s="5" t="s">
+        <v>121</v>
+      </c>
       <c r="F45" s="5"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
@@ -2193,16 +2201,16 @@
     </row>
     <row r="46" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="B46" s="5">
-        <v>0</v>
+        <v>129</v>
+      </c>
+      <c r="B46" s="5" t="s">
+        <v>69</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D46" s="5">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E46" s="5"/>
       <c r="F46" s="5"/>
@@ -2213,38 +2221,36 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="B47" s="5" t="s">
-        <v>56</v>
+        <v>132</v>
+      </c>
+      <c r="B47" s="5">
+        <v>0.01</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="D47" s="5">
-        <v>3</v>
-      </c>
-      <c r="E47" s="5" t="s">
-        <v>128</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="E47" s="5"/>
       <c r="F47" s="5"/>
       <c r="G47" s="5"/>
       <c r="H47" s="5"/>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
     </row>
-    <row r="48" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>137</v>
+        <v>88</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>72</v>
+        <v>89</v>
       </c>
       <c r="C48" s="5" t="s">
         <v>21</v>
       </c>
       <c r="D48" s="5">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="E48" s="5"/>
       <c r="F48" s="5"/>
@@ -2255,16 +2261,16 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="B49" s="5">
-        <v>0.01</v>
+        <v>272</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>273</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>71</v>
+        <v>21</v>
       </c>
       <c r="D49" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
@@ -2273,316 +2279,336 @@
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>94</v>
+        <v>122</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>95</v>
+        <v>37</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="D50" s="5">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E50" s="5"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="5"/>
-      <c r="H50" s="5"/>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
+      <c r="F50" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>174</v>
+      </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="C51" s="5" t="s">
-        <v>21</v>
+        <v>72</v>
       </c>
       <c r="D51" s="5">
         <v>1</v>
       </c>
-      <c r="E51" s="5"/>
-      <c r="F51" s="5"/>
-      <c r="G51" s="5"/>
-      <c r="H51" s="5"/>
-      <c r="I51" s="5"/>
-      <c r="J51" s="5"/>
-    </row>
-    <row r="52" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="E51" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="J51" s="5" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>40</v>
+        <v>91</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
       <c r="D52" s="5">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E52" s="5"/>
       <c r="F52" s="5" t="s">
-        <v>179</v>
+        <v>149</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>180</v>
+        <v>150</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>181</v>
+        <v>151</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>182</v>
+        <v>152</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>183</v>
+        <v>153</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>73</v>
+        <v>24</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>74</v>
+        <v>25</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>75</v>
+        <v>26</v>
       </c>
       <c r="D53" s="5">
         <v>1</v>
       </c>
-      <c r="E53" s="5" t="s">
-        <v>128</v>
-      </c>
+      <c r="E53" s="5"/>
       <c r="F53" s="5" t="s">
-        <v>242</v>
+        <v>138</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>243</v>
+        <v>139</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>244</v>
+        <v>143</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>245</v>
+        <v>140</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>246</v>
+        <v>141</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>121</v>
+        <v>29</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>98</v>
+        <v>30</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="D54" s="5">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E54" s="5"/>
       <c r="F54" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="H54" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="G54" s="5" t="s">
+      <c r="I54" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="J54" s="5" t="s">
         <v>159</v>
-      </c>
-      <c r="H54" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="I54" s="5" t="s">
-        <v>161</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>25</v>
+        <v>224</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>27</v>
-      </c>
+        <v>229</v>
+      </c>
+      <c r="C55" s="5"/>
       <c r="D55" s="5">
         <v>1</v>
       </c>
-      <c r="E55" s="5"/>
+      <c r="E55" s="5" t="s">
+        <v>121</v>
+      </c>
       <c r="F55" s="5" t="s">
-        <v>147</v>
+        <v>230</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>148</v>
+        <v>229</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>152</v>
+        <v>231</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>149</v>
+        <v>220</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>150</v>
+        <v>232</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="D56" s="5">
         <v>1</v>
       </c>
       <c r="E56" s="5"/>
       <c r="F56" s="5" t="s">
-        <v>164</v>
+        <v>190</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>165</v>
+        <v>199</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>167</v>
+        <v>200</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>166</v>
+        <v>201</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>168</v>
+        <v>202</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>233</v>
+        <v>50</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>238</v>
-      </c>
-      <c r="C57" s="5"/>
+        <v>51</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="D57" s="5">
         <v>1</v>
       </c>
-      <c r="E57" s="5" t="s">
-        <v>128</v>
-      </c>
+      <c r="E57" s="5"/>
       <c r="F57" s="5" t="s">
-        <v>239</v>
+        <v>203</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>238</v>
+        <v>51</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>240</v>
+        <v>221</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>241</v>
+        <v>219</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D58" s="5">
         <v>1</v>
       </c>
       <c r="E58" s="5"/>
       <c r="F58" s="5" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>210</v>
+        <v>197</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>211</v>
+        <v>198</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>53</v>
+        <v>73</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>54</v>
+        <v>74</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D59" s="5">
         <v>1</v>
       </c>
       <c r="E59" s="5"/>
       <c r="F59" s="5" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>54</v>
+        <v>191</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>230</v>
+        <v>192</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>229</v>
+        <v>193</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>228</v>
+        <v>194</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>59</v>
+        <v>83</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>60</v>
+        <v>84</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>52</v>
+        <v>85</v>
       </c>
       <c r="D60" s="5">
         <v>1</v>
       </c>
       <c r="E60" s="5"/>
       <c r="F60" s="5" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>204</v>
+        <v>186</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>207</v>
+        <v>189</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
@@ -2590,112 +2616,82 @@
         <v>76</v>
       </c>
       <c r="B61" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="C61" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="C61" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="D61" s="5">
         <v>1</v>
       </c>
       <c r="E61" s="5"/>
       <c r="F61" s="5" t="s">
-        <v>199</v>
+        <v>154</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>200</v>
+        <v>225</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>201</v>
+        <v>226</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>202</v>
+        <v>227</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>203</v>
+        <v>228</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>86</v>
+        <v>264</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>87</v>
+        <v>265</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="D62" s="5">
         <v>1</v>
       </c>
       <c r="E62" s="5"/>
       <c r="F62" s="5" t="s">
-        <v>194</v>
+        <v>155</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>195</v>
+        <v>266</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>197</v>
+        <v>267</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>196</v>
+        <v>268</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>198</v>
+        <v>269</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>79</v>
+        <v>137</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>232</v>
+        <v>22</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>80</v>
+        <v>23</v>
       </c>
       <c r="D63" s="5">
-        <v>1</v>
-      </c>
-      <c r="E63" s="5"/>
-      <c r="F63" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="G63" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="H63" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="I63" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="J63" s="5" t="s">
-        <v>237</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A64" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="B64" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D64" s="5">
         <v>2</v>
       </c>
-      <c r="E64" s="5" t="s">
-        <v>128</v>
-      </c>
-      <c r="F64" s="5"/>
-      <c r="G64" s="5"/>
-      <c r="H64" s="5"/>
-      <c r="I64" s="5"/>
-      <c r="J64" s="5"/>
+      <c r="E63" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="F63" s="5"/>
+      <c r="G63" s="5"/>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
     </row>
   </sheetData>
   <sortState ref="A9:J60">

</xml_diff>

<commit_message>
fix parts missing from bom (using pos export) and fill in passive part nos
</commit_message>
<xml_diff>
--- a/pcb/labio.bom.xlsx
+++ b/pcb/labio.bom.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="460" windowWidth="32560" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="980" yWindow="460" windowWidth="21740" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="labio.bom" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="312">
   <si>
     <t>Source</t>
   </si>
@@ -68,9 +68,6 @@
     <t>Footprint</t>
   </si>
   <si>
-    <t>P1</t>
-  </si>
-  <si>
     <t>CONN_02X20</t>
   </si>
   <si>
@@ -374,9 +371,6 @@
     <t>SW801, SW802, SW803, SW804, SW805</t>
   </si>
   <si>
-    <t>C201, C202, C301, C502, C503, C504, C506, C510, C511, C601, C602, C605, C606, C607, C701, C703, C705, C707, C708, C710, C713, C717</t>
-  </si>
-  <si>
     <t>C801, C802, C803, C804, C805</t>
   </si>
   <si>
@@ -839,9 +833,6 @@
     <t>http://www.digikey.com/product-detail/en/texas-instruments/OPA344NA-250/OPA344NACT-ND/362263</t>
   </si>
   <si>
-    <t>C711, C704,  C719, C720</t>
-  </si>
-  <si>
     <t>R303, R304, R601, R602, R704, R705, R706</t>
   </si>
   <si>
@@ -855,6 +846,123 @@
   </si>
   <si>
     <t>R401, R402, R403, R502, R504, R506, R507, R508, R509, R510, R511, R513, R515</t>
+  </si>
+  <si>
+    <t>C513</t>
+  </si>
+  <si>
+    <t>0.22uF</t>
+  </si>
+  <si>
+    <t>C704, C711,  C719, C720</t>
+  </si>
+  <si>
+    <t>C201, C202, C301, C502, C503, C504, C506, C510, C511, C601, C602, C605, C606, C607, C701, C703, C705, C707, C708, C710, C713, C717, C721</t>
+  </si>
+  <si>
+    <t>labio-special:OMNI-BLOCK_Fuse_10x5mm_Littelfuse</t>
+  </si>
+  <si>
+    <t>P201</t>
+  </si>
+  <si>
+    <t>SMT</t>
+  </si>
+  <si>
+    <t>Murata</t>
+  </si>
+  <si>
+    <t>GRM188R71C104KA01D</t>
+  </si>
+  <si>
+    <t>CAP CER 0.1uF ±10% 16V X7R 0603</t>
+  </si>
+  <si>
+    <t>GRM188R71H103KA01D</t>
+  </si>
+  <si>
+    <t>CAP CER 0.01uF ±10% 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>GRM188R71C224KA01D</t>
+  </si>
+  <si>
+    <t>CAP CER 0.22UF ±10% 16V X7R 0603</t>
+  </si>
+  <si>
+    <t>GRM188R71H221KA01D</t>
+  </si>
+  <si>
+    <t>CAP CER 220PF ±10% 50V X7R 0603</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>CRCW06032K20FKEA</t>
+  </si>
+  <si>
+    <t>RES SMD 2.2K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>CRCW0603220RFKEA</t>
+  </si>
+  <si>
+    <t>RES SMD 220 OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>CRCW060310K0FKEA</t>
+  </si>
+  <si>
+    <t>RES SMD 10K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>CRCW06030000Z0EA</t>
+  </si>
+  <si>
+    <t>RES SMD 0.0OHM JUMPER 1/10W 0603</t>
+  </si>
+  <si>
+    <t>CRCW060320K0FKEA</t>
+  </si>
+  <si>
+    <t>RES SMD 20K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>CRCW060347K0FKEA</t>
+  </si>
+  <si>
+    <t>RES SMD 47K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>CRCW0603820KFKEA</t>
+  </si>
+  <si>
+    <t>RES SMD 820K OHM 1% 1/10W 0603</t>
+  </si>
+  <si>
+    <t>RUW3216FR100CS</t>
+  </si>
+  <si>
+    <t>RES SMD 0.1 OHM 1% 1W 1206</t>
+  </si>
+  <si>
+    <t>1276-6187-1-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/RUW3216FR100CS/1276-6187-1-ND/3969159</t>
+  </si>
+  <si>
+    <t>CL10B105KP8NNNC</t>
+  </si>
+  <si>
+    <t>1µF 10V Ceramic Capacitor X7R 0603 (1608 Metric) 0.063" L x 0.031" W (1.60mm x 0.80mm)</t>
+  </si>
+  <si>
+    <t>1276-1946-1-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/CL10B105KP8NNNC/1276-1946-1-ND/3890032</t>
   </si>
 </sst>
 </file>
@@ -1204,11 +1312,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:J64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1244,7 +1352,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1290,448 +1398,508 @@
         <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>142</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>115</v>
+        <v>276</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>28</v>
-      </c>
       <c r="D9" s="5">
-        <v>22</v>
-      </c>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
+        <v>23</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>282</v>
+      </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="D10" s="5">
         <v>10</v>
       </c>
-      <c r="E10" s="5"/>
+      <c r="E10" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="F10" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="H10" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="I10" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>216</v>
-      </c>
-      <c r="I10" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>55</v>
-      </c>
       <c r="C11" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" s="5">
         <v>1</v>
       </c>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
+      <c r="E11" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>284</v>
+      </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>118</v>
+        <v>273</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>64</v>
+        <v>274</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>65</v>
+        <v>27</v>
       </c>
       <c r="D12" s="5">
-        <v>4</v>
-      </c>
-      <c r="E12" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="F12" s="5" t="s">
-        <v>209</v>
+        <v>280</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>210</v>
+        <v>285</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>211</v>
-      </c>
-      <c r="I12" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>213</v>
-      </c>
+        <v>286</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>257</v>
+        <v>116</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>86</v>
+        <v>63</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="D13" s="5">
-        <v>1</v>
-      </c>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D14" s="5">
-        <v>4</v>
-      </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F14" s="5" t="s">
+        <v>280</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="H14" s="5" t="s">
+        <v>288</v>
+      </c>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>255</v>
+        <v>275</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>256</v>
+        <v>86</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>262</v>
+        <v>27</v>
       </c>
       <c r="D15" s="5">
-        <v>2</v>
-      </c>
-      <c r="E15" s="5"/>
+        <v>4</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="F15" s="5" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>258</v>
+        <v>308</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>259</v>
+        <v>309</v>
       </c>
       <c r="I15" s="5" t="s">
-        <v>260</v>
+        <v>310</v>
       </c>
       <c r="J15" s="5" t="s">
-        <v>261</v>
+        <v>311</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>116</v>
+        <v>253</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>93</v>
+        <v>254</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>28</v>
+        <v>260</v>
       </c>
       <c r="D16" s="5">
+        <v>2</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="I16" s="5" t="s">
+        <v>258</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" s="5">
         <v>5</v>
       </c>
-      <c r="E16" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="5"/>
-      <c r="J16" s="5"/>
-    </row>
-    <row r="17" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D17" s="5">
+      <c r="E17" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="5">
         <v>19</v>
       </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5" t="s">
+      <c r="E18" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F18" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="H18" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="I18" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="J18" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="I17" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B18" s="5" t="s">
+    </row>
+    <row r="19" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D18" s="5">
+      <c r="D19" s="5">
         <v>12</v>
       </c>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5" t="s">
+      <c r="E19" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="H19" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="I19" s="5" t="s">
         <v>145</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="J19" s="5" t="s">
         <v>146</v>
-      </c>
-      <c r="I18" s="5" t="s">
-        <v>147</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="5">
-        <v>6</v>
-      </c>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="G19" s="5" t="s">
-        <v>249</v>
-      </c>
-      <c r="H19" s="5" t="s">
-        <v>246</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>238</v>
+        <v>261</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C20" s="5"/>
+        <v>237</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="D20" s="5">
-        <v>1</v>
-      </c>
-      <c r="E20" s="5"/>
+        <v>6</v>
+      </c>
+      <c r="E20" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="F20" s="5" t="s">
-        <v>241</v>
+        <v>248</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>242</v>
+        <v>247</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="I20" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="J20" s="5" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="G21" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>239</v>
-      </c>
-      <c r="C21" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="D21" s="5">
-        <v>1</v>
-      </c>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5" t="s">
-        <v>250</v>
-      </c>
-      <c r="G21" s="5" t="s">
-        <v>251</v>
-      </c>
       <c r="H21" s="5" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>104</v>
+        <v>238</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>105</v>
+        <v>237</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>106</v>
+        <v>67</v>
       </c>
       <c r="D22" s="5">
         <v>1</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="5"/>
+        <v>279</v>
+      </c>
+      <c r="F22" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="I22" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="D23" s="5">
         <v>1</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
-      <c r="H23" s="6"/>
+      <c r="H23" s="5"/>
       <c r="I23" s="5"/>
       <c r="J23" s="5"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D24" s="5">
         <v>1</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="5"/>
+      <c r="H24" s="6"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>103</v>
+        <v>107</v>
       </c>
       <c r="D25" s="5">
         <v>1</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -1739,21 +1907,21 @@
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="D26" s="5">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
@@ -1761,21 +1929,21 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>16</v>
+        <v>121</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>17</v>
+        <v>96</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>18</v>
+        <v>97</v>
       </c>
       <c r="D27" s="5">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -1785,69 +1953,73 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>81</v>
+        <v>16</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>82</v>
+        <v>17</v>
       </c>
       <c r="D28" s="5">
         <v>1</v>
       </c>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="G28" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="H28" s="5" t="s">
-        <v>167</v>
-      </c>
-      <c r="I28" s="5" t="s">
-        <v>168</v>
-      </c>
-      <c r="J28" s="5" t="s">
-        <v>169</v>
-      </c>
+      <c r="E28" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>13</v>
+        <v>79</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>14</v>
+        <v>80</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="D29" s="5">
         <v>1</v>
       </c>
-      <c r="E29" s="5"/>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
+      <c r="E29" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F29" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="I29" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>167</v>
+      </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>127</v>
+        <v>278</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>33</v>
+        <v>14</v>
       </c>
       <c r="D30" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -1857,71 +2029,73 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>42</v>
+        <v>125</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="D31" s="5">
-        <v>1</v>
-      </c>
-      <c r="E31" s="5"/>
-      <c r="F31" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="G31" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>177</v>
-      </c>
-      <c r="I31" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>179</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="E31" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5"/>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>125</v>
+        <v>41</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="D32" s="5">
         <v>1</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
+        <v>279</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="I32" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D33" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
@@ -1931,19 +2105,19 @@
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="D34" s="5">
         <v>2</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
@@ -1953,19 +2127,19 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>78</v>
+        <v>126</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>79</v>
+        <v>60</v>
       </c>
       <c r="D35" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
@@ -1975,19 +2149,19 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>94</v>
+        <v>77</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>95</v>
+        <v>61</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>96</v>
+        <v>78</v>
       </c>
       <c r="D36" s="5">
         <v>1</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
@@ -1997,701 +2171,825 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D37" s="5">
+        <v>1</v>
+      </c>
+      <c r="E37" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5"/>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A38" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B37" s="5" t="s">
+      <c r="C38" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="D37" s="5">
-        <v>1</v>
-      </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="5" t="s">
+      <c r="D38" s="5">
+        <v>1</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="H38" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="G37" s="5" t="s">
+      <c r="I38" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="H37" s="5" t="s">
+      <c r="J38" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="I37" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="J37" s="5" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A38" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="B38" s="5" t="s">
+    </row>
+    <row r="39" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38" s="5">
+      <c r="D39" s="5">
         <v>15</v>
       </c>
-      <c r="E38" s="5"/>
-      <c r="F38" s="5" t="s">
+      <c r="E39" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="H39" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="I39" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="J39" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="I38" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="J38" s="5" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
-        <v>274</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="C39" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D39" s="5">
-        <v>4</v>
-      </c>
-      <c r="E39" s="5"/>
-      <c r="F39" s="5"/>
-      <c r="G39" s="5"/>
-      <c r="H39" s="5"/>
-      <c r="I39" s="5"/>
-      <c r="J39" s="5"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>19</v>
+        <v>271</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>134</v>
+        <v>89</v>
       </c>
       <c r="C40" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D40" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F40" s="5"/>
-      <c r="G40" s="5"/>
-      <c r="H40" s="5"/>
+        <v>279</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>291</v>
+      </c>
       <c r="I40" s="5"/>
       <c r="J40" s="5"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>136</v>
+        <v>18</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D41" s="5">
-        <v>2</v>
-      </c>
-      <c r="E41" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="E41" s="5" t="s">
+        <v>119</v>
+      </c>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B42" s="5">
-        <v>220</v>
+        <v>134</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>133</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D42" s="5">
-        <v>19</v>
-      </c>
-      <c r="E42" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="E42" s="5" t="s">
+        <v>119</v>
+      </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="B43" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="B43" s="5">
+        <v>220</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C43" s="5" t="s">
-        <v>21</v>
-      </c>
       <c r="D43" s="5">
-        <v>7</v>
-      </c>
-      <c r="E43" s="5"/>
-      <c r="F43" s="5"/>
-      <c r="G43" s="5"/>
-      <c r="H43" s="5"/>
+        <v>19</v>
+      </c>
+      <c r="E43" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F43" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="H43" s="5" t="s">
+        <v>293</v>
+      </c>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>275</v>
-      </c>
-      <c r="B44" s="5">
-        <v>0</v>
+        <v>268</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D44" s="5">
-        <v>13</v>
-      </c>
-      <c r="E44" s="5"/>
-      <c r="F44" s="5"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="5"/>
+        <v>7</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>295</v>
+      </c>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B45" s="5" t="s">
-        <v>53</v>
+        <v>272</v>
+      </c>
+      <c r="B45" s="5">
+        <v>0</v>
       </c>
       <c r="C45" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D45" s="5">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F45" s="5"/>
-      <c r="G45" s="5"/>
-      <c r="H45" s="5"/>
+        <v>279</v>
+      </c>
+      <c r="F45" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="H45" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
     </row>
-    <row r="46" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
         <v>129</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D46" s="5">
-        <v>15</v>
-      </c>
-      <c r="E46" s="5"/>
-      <c r="F46" s="5"/>
-      <c r="G46" s="5"/>
-      <c r="H46" s="5"/>
+        <v>3</v>
+      </c>
+      <c r="E46" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F46" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="G46" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="H46" s="5" t="s">
+        <v>297</v>
+      </c>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>132</v>
-      </c>
-      <c r="B47" s="5">
-        <v>0.01</v>
+        <v>127</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>68</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="D47" s="5">
-        <v>2</v>
-      </c>
-      <c r="E47" s="5"/>
-      <c r="F47" s="5"/>
-      <c r="G47" s="5"/>
-      <c r="H47" s="5"/>
+        <v>15</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>299</v>
+      </c>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B48" s="5" t="s">
-        <v>89</v>
+        <v>130</v>
+      </c>
+      <c r="B48" s="5">
+        <v>0.01</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="D48" s="5">
-        <v>1</v>
-      </c>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5"/>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5"/>
-      <c r="I48" s="5"/>
-      <c r="J48" s="5"/>
+        <v>2</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>272</v>
+        <v>87</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>273</v>
+        <v>88</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D49" s="5">
         <v>1</v>
       </c>
-      <c r="E49" s="5"/>
-      <c r="F49" s="5"/>
-      <c r="G49" s="5"/>
-      <c r="H49" s="5"/>
+      <c r="E49" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>301</v>
+      </c>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
     </row>
-    <row r="50" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>122</v>
+        <v>269</v>
       </c>
       <c r="B50" s="5" t="s">
+        <v>270</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D50" s="5">
+        <v>1</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="I50" s="5"/>
+      <c r="J50" s="5"/>
+    </row>
+    <row r="51" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C50" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D50" s="5">
+      <c r="D51" s="5">
         <v>10</v>
       </c>
-      <c r="E50" s="5"/>
-      <c r="F50" s="5" t="s">
+      <c r="E51" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="H51" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="G50" s="5" t="s">
+      <c r="I51" s="5" t="s">
         <v>171</v>
       </c>
-      <c r="H50" s="5" t="s">
+      <c r="J51" s="5" t="s">
         <v>172</v>
-      </c>
-      <c r="I50" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="J50" s="5" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="D51" s="5">
-        <v>1</v>
-      </c>
-      <c r="E51" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F51" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="G51" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="H51" s="5" t="s">
-        <v>235</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>236</v>
-      </c>
-      <c r="J51" s="5" t="s">
-        <v>237</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>114</v>
+        <v>69</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="D52" s="5">
-        <v>5</v>
-      </c>
-      <c r="E52" s="5"/>
+        <v>1</v>
+      </c>
+      <c r="E52" s="5" t="s">
+        <v>119</v>
+      </c>
       <c r="F52" s="5" t="s">
-        <v>149</v>
+        <v>231</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>150</v>
+        <v>232</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>151</v>
+        <v>233</v>
       </c>
       <c r="I52" s="5" t="s">
-        <v>152</v>
+        <v>234</v>
       </c>
       <c r="J52" s="5" t="s">
-        <v>153</v>
+        <v>235</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>24</v>
+        <v>113</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>25</v>
+        <v>90</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>26</v>
+        <v>91</v>
       </c>
       <c r="D53" s="5">
-        <v>1</v>
-      </c>
-      <c r="E53" s="5"/>
+        <v>5</v>
+      </c>
+      <c r="E53" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="F53" s="5" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>143</v>
+        <v>149</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>141</v>
+        <v>151</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D54" s="5">
         <v>1</v>
       </c>
-      <c r="E54" s="5"/>
+      <c r="E54" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="F54" s="5" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>156</v>
+        <v>137</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>158</v>
+        <v>141</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>157</v>
+        <v>138</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>224</v>
+        <v>28</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="C55" s="5"/>
+        <v>29</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="D55" s="5">
         <v>1</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>121</v>
+        <v>279</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>230</v>
+        <v>153</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>229</v>
+        <v>154</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>231</v>
+        <v>156</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>220</v>
+        <v>155</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>232</v>
+        <v>157</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>47</v>
+        <v>222</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>49</v>
-      </c>
+        <v>227</v>
+      </c>
+      <c r="C56" s="5"/>
       <c r="D56" s="5">
         <v>1</v>
       </c>
-      <c r="E56" s="5"/>
+      <c r="E56" s="5" t="s">
+        <v>119</v>
+      </c>
       <c r="F56" s="5" t="s">
-        <v>190</v>
+        <v>228</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>199</v>
+        <v>227</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>200</v>
+        <v>229</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>202</v>
+        <v>230</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D57" s="5">
         <v>1</v>
       </c>
-      <c r="E57" s="5"/>
+      <c r="E57" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="F57" s="5" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>51</v>
+        <v>197</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>219</v>
+        <v>200</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D58" s="5">
         <v>1</v>
       </c>
-      <c r="E58" s="5"/>
+      <c r="E58" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="F58" s="5" t="s">
-        <v>190</v>
+        <v>201</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>195</v>
+        <v>50</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>196</v>
+        <v>219</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>197</v>
+        <v>218</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>198</v>
+        <v>217</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
       <c r="D59" s="5">
         <v>1</v>
       </c>
-      <c r="E59" s="5"/>
+      <c r="E59" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="F59" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>192</v>
+        <v>194</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>194</v>
+        <v>196</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="D60" s="5">
         <v>1</v>
       </c>
-      <c r="E60" s="5"/>
+      <c r="E60" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="F60" s="5" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>223</v>
+        <v>83</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>77</v>
+        <v>84</v>
       </c>
       <c r="D61" s="5">
         <v>1</v>
       </c>
-      <c r="E61" s="5"/>
+      <c r="E61" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="F61" s="5" t="s">
-        <v>154</v>
+        <v>183</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>225</v>
+        <v>184</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>226</v>
+        <v>186</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>227</v>
+        <v>185</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>228</v>
+        <v>187</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>264</v>
+        <v>75</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>265</v>
+        <v>221</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>26</v>
+        <v>76</v>
       </c>
       <c r="D62" s="5">
         <v>1</v>
       </c>
-      <c r="E62" s="5"/>
+      <c r="E62" s="5" t="s">
+        <v>279</v>
+      </c>
       <c r="F62" s="5" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>266</v>
+        <v>223</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>267</v>
+        <v>224</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>268</v>
+        <v>225</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>269</v>
+        <v>226</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>137</v>
+        <v>262</v>
       </c>
       <c r="B63" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D63" s="5">
+        <v>1</v>
+      </c>
+      <c r="E63" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="F63" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="H63" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="I63" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="J63" s="5" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="C64" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="D63" s="5">
+      <c r="D64" s="5">
         <v>2</v>
       </c>
-      <c r="E63" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="F63" s="5"/>
-      <c r="G63" s="5"/>
-      <c r="H63" s="5"/>
-      <c r="I63" s="5"/>
-      <c r="J63" s="5"/>
+      <c r="E64" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F64" s="5"/>
+      <c r="G64" s="5"/>
+      <c r="H64" s="5"/>
+      <c r="I64" s="5"/>
+      <c r="J64" s="5"/>
     </row>
   </sheetData>
   <sortState ref="A9:J60">

</xml_diff>

<commit_message>
add options for driving oled reset. no changes to stuffed bom parts.
</commit_message>
<xml_diff>
--- a/pcb/labio.bom.xlsx
+++ b/pcb/labio.bom.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="980" yWindow="460" windowWidth="21740" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="1040" yWindow="460" windowWidth="21740" windowHeight="20540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="labio.bom" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="316">
   <si>
     <t>Source</t>
   </si>
@@ -416,9 +416,6 @@
     <t>R302, R501, R605, R606, R607, R612, R613, R618, R619, R622, R623, R624, R626, R627, R630, R631, R634, R635, R701</t>
   </si>
   <si>
-    <t>R503, R512, R514</t>
-  </si>
-  <si>
     <t>R614, R615</t>
   </si>
   <si>
@@ -963,6 +960,21 @@
   </si>
   <si>
     <t>http://www.digikey.com/product-detail/en/samsung-electro-mechanics-america-inc/CL10B105KP8NNNC/1276-1946-1-ND/3890032</t>
+  </si>
+  <si>
+    <t>C401</t>
+  </si>
+  <si>
+    <t>dnp-4.7uF</t>
+  </si>
+  <si>
+    <t>R405</t>
+  </si>
+  <si>
+    <t>dnp-47k</t>
+  </si>
+  <si>
+    <t>R404, R406, R503, R512, R514</t>
   </si>
 </sst>
 </file>
@@ -1312,11 +1324,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J64"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <pane ySplit="8" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1352,7 +1364,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1410,7 +1422,7 @@
         <v>110</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I8" s="3" t="s">
         <v>111</v>
@@ -1421,7 +1433,7 @@
     </row>
     <row r="9" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>26</v>
@@ -1433,86 +1445,90 @@
         <v>23</v>
       </c>
       <c r="E9" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>280</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>281</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>282</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="10" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>115</v>
+        <v>311</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>44</v>
+        <v>312</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D10" s="5">
+        <v>1</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="H10" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="5">
         <v>10</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="F10" s="5" t="s">
+      <c r="E11" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>214</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="J11" s="5" t="s">
         <v>215</v>
       </c>
-      <c r="J10" s="5" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" s="5">
-        <v>1</v>
-      </c>
-      <c r="E11" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="F11" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="H11" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>273</v>
+        <v>53</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>274</v>
+        <v>54</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>27</v>
@@ -1521,357 +1537,363 @@
         <v>1</v>
       </c>
       <c r="E12" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>280</v>
-      </c>
       <c r="G12" s="5" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>116</v>
+        <v>272</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>63</v>
+        <v>273</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>64</v>
+        <v>27</v>
       </c>
       <c r="D13" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E13" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>207</v>
-      </c>
       <c r="G13" s="5" t="s">
-        <v>208</v>
+        <v>284</v>
       </c>
       <c r="H13" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="I13" s="5" t="s">
-        <v>210</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>211</v>
-      </c>
+        <v>285</v>
+      </c>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>255</v>
+        <v>116</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>27</v>
+        <v>64</v>
       </c>
       <c r="D14" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>280</v>
+        <v>206</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>287</v>
+        <v>207</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>288</v>
-      </c>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
+        <v>208</v>
+      </c>
+      <c r="I14" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>275</v>
+        <v>254</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>27</v>
       </c>
       <c r="D15" s="5">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E15" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>212</v>
-      </c>
       <c r="G15" s="5" t="s">
-        <v>308</v>
+        <v>286</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>309</v>
-      </c>
-      <c r="I15" s="5" t="s">
-        <v>310</v>
-      </c>
-      <c r="J15" s="5" t="s">
-        <v>311</v>
-      </c>
+        <v>287</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>253</v>
+        <v>274</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>254</v>
+        <v>86</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>260</v>
+        <v>27</v>
       </c>
       <c r="D16" s="5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>256</v>
+        <v>307</v>
       </c>
       <c r="H16" s="5" t="s">
-        <v>257</v>
+        <v>308</v>
       </c>
       <c r="I16" s="5" t="s">
-        <v>258</v>
+        <v>309</v>
       </c>
       <c r="J16" s="5" t="s">
-        <v>259</v>
+        <v>310</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>259</v>
+      </c>
+      <c r="D17" s="5">
+        <v>2</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>256</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>257</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B18" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C18" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D18" s="5">
         <v>5</v>
       </c>
-      <c r="E17" s="5" t="s">
+      <c r="E18" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-    </row>
-    <row r="18" spans="1:10" ht="48" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B19" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C19" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D18" s="5">
+      <c r="D19" s="5">
         <v>19</v>
       </c>
-      <c r="E18" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="F18" s="5" t="s">
+      <c r="E19" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="H18" s="5" t="s">
+      <c r="I19" s="5" t="s">
         <v>180</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="J19" s="5" t="s">
         <v>181</v>
       </c>
-      <c r="J18" s="5" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+    </row>
+    <row r="20" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B20" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C19" s="5" t="s">
+      <c r="C20" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="D19" s="5">
+      <c r="D20" s="5">
         <v>12</v>
       </c>
-      <c r="E19" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="F19" s="5" t="s">
+      <c r="E20" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="H20" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="I20" s="5" t="s">
         <v>144</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="J20" s="5" t="s">
         <v>145</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D20" s="5">
-        <v>6</v>
-      </c>
-      <c r="E20" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>248</v>
-      </c>
-      <c r="G20" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="H20" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B21" s="5" t="s">
         <v>236</v>
       </c>
-      <c r="B21" s="5" t="s">
-        <v>237</v>
-      </c>
       <c r="C21" s="5" t="s">
-        <v>277</v>
+        <v>67</v>
       </c>
       <c r="D21" s="5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>239</v>
+        <v>247</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="I21" s="5" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="J21" s="5" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>276</v>
+      </c>
+      <c r="D22" s="5">
+        <v>1</v>
+      </c>
+      <c r="E22" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F22" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="5">
-        <v>1</v>
-      </c>
-      <c r="E22" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>248</v>
-      </c>
       <c r="G22" s="5" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="I22" s="5" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>103</v>
+        <v>237</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>104</v>
+        <v>236</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>105</v>
+        <v>67</v>
       </c>
       <c r="D23" s="5">
         <v>1</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F23" s="5"/>
-      <c r="G23" s="5"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="5"/>
-      <c r="J23" s="5"/>
+        <v>278</v>
+      </c>
+      <c r="F23" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="G23" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="I23" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>251</v>
+      </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="D24" s="5">
         <v>1</v>
@@ -1881,19 +1903,19 @@
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
-      <c r="H24" s="6"/>
+      <c r="H24" s="5"/>
       <c r="I24" s="5"/>
       <c r="J24" s="5"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="D25" s="5">
         <v>1</v>
@@ -1903,19 +1925,19 @@
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
-      <c r="H25" s="5"/>
+      <c r="H25" s="6"/>
       <c r="I25" s="5"/>
       <c r="J25" s="5"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="D26" s="5">
         <v>1</v>
@@ -1929,18 +1951,18 @@
       <c r="I26" s="5"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="D27" s="5">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="E27" s="5" t="s">
         <v>119</v>
@@ -1951,18 +1973,18 @@
       <c r="I27" s="5"/>
       <c r="J27" s="5"/>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>16</v>
+        <v>96</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>17</v>
+        <v>97</v>
       </c>
       <c r="D28" s="5">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="E28" s="5" t="s">
         <v>119</v>
@@ -1975,70 +1997,70 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>79</v>
+        <v>15</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>80</v>
+        <v>16</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>81</v>
+        <v>17</v>
       </c>
       <c r="D29" s="5">
         <v>1</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>163</v>
-      </c>
-      <c r="G29" s="5" t="s">
-        <v>164</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>165</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>166</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>167</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>278</v>
+        <v>79</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>13</v>
+        <v>80</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>14</v>
+        <v>81</v>
       </c>
       <c r="D30" s="5">
         <v>1</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="5"/>
-      <c r="J30" s="5"/>
+        <v>278</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="G30" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>125</v>
+        <v>277</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>31</v>
+        <v>13</v>
       </c>
       <c r="C31" s="5" t="s">
-        <v>32</v>
+        <v>14</v>
       </c>
       <c r="D31" s="5">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="E31" s="5" t="s">
         <v>119</v>
@@ -2051,70 +2073,70 @@
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>41</v>
+        <v>125</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>43</v>
+        <v>32</v>
       </c>
       <c r="D32" s="5">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>173</v>
-      </c>
-      <c r="G32" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="I32" s="5" t="s">
-        <v>176</v>
-      </c>
-      <c r="J32" s="5" t="s">
-        <v>177</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5"/>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>123</v>
+        <v>41</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>61</v>
+        <v>42</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="D33" s="5">
         <v>1</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
+        <v>278</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="I33" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>176</v>
+      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="D34" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E34" s="5" t="s">
         <v>119</v>
@@ -2127,13 +2149,13 @@
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C35" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D35" s="5">
         <v>2</v>
@@ -2149,16 +2171,16 @@
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>77</v>
+        <v>126</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="D36" s="5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E36" s="5" t="s">
         <v>119</v>
@@ -2171,13 +2193,13 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>94</v>
+        <v>61</v>
       </c>
       <c r="C37" s="5" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="D37" s="5">
         <v>1</v>
@@ -2193,130 +2215,130 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D38" s="5">
+        <v>1</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5"/>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A39" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="B39" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="D38" s="5">
-        <v>1</v>
-      </c>
-      <c r="E38" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="F38" s="5" t="s">
+      <c r="D39" s="5">
+        <v>1</v>
+      </c>
+      <c r="E39" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F39" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="G39" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="G38" s="5" t="s">
+      <c r="H39" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="H38" s="5" t="s">
+      <c r="I39" s="5" t="s">
         <v>160</v>
       </c>
-      <c r="I38" s="5" t="s">
+      <c r="J39" s="5" t="s">
         <v>161</v>
       </c>
-      <c r="J38" s="5" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A39" s="4" t="s">
-        <v>131</v>
-      </c>
-      <c r="B39" s="5" t="s">
+    </row>
+    <row r="40" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A40" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="5" t="s">
+      <c r="C40" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D39" s="5">
+      <c r="D40" s="5">
         <v>15</v>
       </c>
-      <c r="E39" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="F39" s="5" t="s">
+      <c r="E40" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="G40" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="G39" s="5" t="s">
+      <c r="H40" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="H39" s="5" t="s">
+      <c r="I40" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="I39" s="5" t="s">
+      <c r="J40" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="J39" s="5" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D40" s="5">
-        <v>4</v>
-      </c>
-      <c r="E40" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="F40" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="G40" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="H40" s="5" t="s">
-        <v>291</v>
-      </c>
-      <c r="I40" s="5"/>
-      <c r="J40" s="5"/>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>18</v>
+        <v>270</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>132</v>
+        <v>89</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D41" s="5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F41" s="5"/>
-      <c r="G41" s="5"/>
-      <c r="H41" s="5"/>
+        <v>278</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="G41" s="5" t="s">
+        <v>289</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>290</v>
+      </c>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>134</v>
+        <v>18</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D42" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E42" s="5" t="s">
         <v>119</v>
@@ -2327,494 +2349,480 @@
       <c r="I42" s="5"/>
       <c r="J42" s="5"/>
     </row>
-    <row r="43" spans="1:10" ht="48" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B43" s="5">
-        <v>220</v>
+        <v>133</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>132</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D43" s="5">
-        <v>19</v>
+        <v>2</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="F43" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="G43" s="5" t="s">
-        <v>292</v>
-      </c>
-      <c r="H43" s="5" t="s">
-        <v>293</v>
-      </c>
+        <v>119</v>
+      </c>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5"/>
       <c r="I43" s="5"/>
       <c r="J43" s="5"/>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>19</v>
+        <v>128</v>
+      </c>
+      <c r="B44" s="5">
+        <v>220</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D44" s="5">
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="H44" s="5" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
     </row>
-    <row r="45" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="B45" s="5">
-        <v>0</v>
+        <v>267</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>19</v>
       </c>
       <c r="C45" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D45" s="5">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="H45" s="5" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>129</v>
-      </c>
-      <c r="B46" s="5" t="s">
-        <v>52</v>
+        <v>271</v>
+      </c>
+      <c r="B46" s="5">
+        <v>0</v>
       </c>
       <c r="C46" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D46" s="5">
-        <v>3</v>
+        <v>13</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>119</v>
+        <v>278</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G46" s="5" t="s">
+        <v>295</v>
+      </c>
+      <c r="H46" s="5" t="s">
         <v>296</v>
-      </c>
-      <c r="H46" s="5" t="s">
-        <v>297</v>
       </c>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
     </row>
-    <row r="47" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>127</v>
+        <v>315</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="C47" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D47" s="5">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>279</v>
+        <v>119</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="H47" s="5" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="B48" s="5">
-        <v>0.01</v>
+        <v>313</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>314</v>
       </c>
       <c r="C48" s="5" t="s">
-        <v>67</v>
+        <v>20</v>
       </c>
       <c r="D48" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>279</v>
+        <v>119</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>212</v>
+        <v>288</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="H48" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="I48" s="5" t="s">
-        <v>306</v>
-      </c>
-      <c r="J48" s="5" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
+        <v>300</v>
+      </c>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5"/>
+    </row>
+    <row r="49" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>87</v>
+        <v>127</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>20</v>
       </c>
       <c r="D49" s="5">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="H49" s="5" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="B50" s="5" t="s">
-        <v>270</v>
+        <v>129</v>
+      </c>
+      <c r="B50" s="5">
+        <v>0.01</v>
       </c>
       <c r="C50" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D50" s="5">
+        <v>2</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>304</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A51" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C51" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D50" s="5">
-        <v>1</v>
-      </c>
-      <c r="E50" s="5" t="s">
-        <v>279</v>
-      </c>
-      <c r="F50" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="G50" s="5" t="s">
-        <v>302</v>
-      </c>
-      <c r="H50" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="I50" s="5"/>
-      <c r="J50" s="5"/>
-    </row>
-    <row r="51" spans="1:10" ht="32" x14ac:dyDescent="0.2">
-      <c r="A51" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B51" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="C51" s="5" t="s">
-        <v>37</v>
-      </c>
       <c r="D51" s="5">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>168</v>
+        <v>288</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>169</v>
+        <v>299</v>
       </c>
       <c r="H51" s="5" t="s">
-        <v>170</v>
-      </c>
-      <c r="I51" s="5" t="s">
-        <v>171</v>
-      </c>
-      <c r="J51" s="5" t="s">
-        <v>172</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="I51" s="5"/>
+      <c r="J51" s="5"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>69</v>
+        <v>268</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>70</v>
+        <v>269</v>
       </c>
       <c r="C52" s="5" t="s">
-        <v>71</v>
+        <v>20</v>
       </c>
       <c r="D52" s="5">
         <v>1</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>119</v>
+        <v>278</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>231</v>
+        <v>288</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>232</v>
+        <v>301</v>
       </c>
       <c r="H52" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="I52" s="5" t="s">
-        <v>234</v>
-      </c>
-      <c r="J52" s="5" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
+        <v>302</v>
+      </c>
+      <c r="I52" s="5"/>
+      <c r="J52" s="5"/>
+    </row>
+    <row r="53" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>90</v>
+        <v>36</v>
       </c>
       <c r="C53" s="5" t="s">
-        <v>91</v>
+        <v>37</v>
       </c>
       <c r="D53" s="5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="H53" s="5" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="I53" s="5" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="J53" s="5" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="D54" s="5">
         <v>1</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>279</v>
+        <v>119</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>136</v>
+        <v>230</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>137</v>
+        <v>231</v>
       </c>
       <c r="H54" s="5" t="s">
-        <v>141</v>
+        <v>232</v>
       </c>
       <c r="I54" s="5" t="s">
-        <v>138</v>
+        <v>233</v>
       </c>
       <c r="J54" s="5" t="s">
-        <v>139</v>
+        <v>234</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>28</v>
+        <v>113</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>29</v>
+        <v>90</v>
       </c>
       <c r="C55" s="5" t="s">
-        <v>30</v>
+        <v>91</v>
       </c>
       <c r="D55" s="5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="H55" s="5" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="I55" s="5" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
       <c r="J55" s="5" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>222</v>
+        <v>23</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>227</v>
-      </c>
-      <c r="C56" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>25</v>
+      </c>
       <c r="D56" s="5">
         <v>1</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>119</v>
+        <v>278</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>228</v>
+        <v>135</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>227</v>
+        <v>136</v>
       </c>
       <c r="H56" s="5" t="s">
-        <v>229</v>
+        <v>140</v>
       </c>
       <c r="I56" s="5" t="s">
-        <v>218</v>
+        <v>137</v>
       </c>
       <c r="J56" s="5" t="s">
-        <v>230</v>
+        <v>138</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="D57" s="5">
         <v>1</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>188</v>
+        <v>152</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>197</v>
+        <v>153</v>
       </c>
       <c r="H57" s="5" t="s">
-        <v>198</v>
+        <v>155</v>
       </c>
       <c r="I57" s="5" t="s">
-        <v>199</v>
+        <v>154</v>
       </c>
       <c r="J57" s="5" t="s">
-        <v>200</v>
+        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>49</v>
+        <v>221</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>51</v>
-      </c>
+        <v>226</v>
+      </c>
+      <c r="C58" s="5"/>
       <c r="D58" s="5">
         <v>1</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>279</v>
+        <v>119</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>201</v>
+        <v>227</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>50</v>
+        <v>226</v>
       </c>
       <c r="H58" s="5" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
       <c r="I58" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J58" s="5" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="C59" s="5" t="s">
         <v>48</v>
@@ -2823,173 +2831,237 @@
         <v>1</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="H59" s="5" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="I59" s="5" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="J59" s="5" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>72</v>
+        <v>49</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>73</v>
+        <v>50</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>74</v>
+        <v>51</v>
       </c>
       <c r="D60" s="5">
         <v>1</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>188</v>
+        <v>200</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>189</v>
+        <v>50</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>190</v>
+        <v>218</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>191</v>
+        <v>217</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>192</v>
+        <v>216</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>82</v>
+        <v>55</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>83</v>
+        <v>56</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>84</v>
+        <v>48</v>
       </c>
       <c r="D61" s="5">
         <v>1</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>184</v>
+        <v>192</v>
       </c>
       <c r="H61" s="5" t="s">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="I61" s="5" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="J61" s="5" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>221</v>
+        <v>73</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D62" s="5">
         <v>1</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>152</v>
+        <v>187</v>
       </c>
       <c r="G62" s="5" t="s">
-        <v>223</v>
+        <v>188</v>
       </c>
       <c r="H62" s="5" t="s">
-        <v>224</v>
+        <v>189</v>
       </c>
       <c r="I62" s="5" t="s">
-        <v>225</v>
+        <v>190</v>
       </c>
       <c r="J62" s="5" t="s">
-        <v>226</v>
+        <v>191</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>262</v>
+        <v>82</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>263</v>
+        <v>83</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>25</v>
+        <v>84</v>
       </c>
       <c r="D63" s="5">
         <v>1</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>153</v>
+        <v>182</v>
       </c>
       <c r="G63" s="5" t="s">
-        <v>264</v>
+        <v>183</v>
       </c>
       <c r="H63" s="5" t="s">
-        <v>265</v>
+        <v>185</v>
       </c>
       <c r="I63" s="5" t="s">
-        <v>266</v>
+        <v>184</v>
       </c>
       <c r="J63" s="5" t="s">
-        <v>267</v>
+        <v>186</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>135</v>
+        <v>75</v>
       </c>
       <c r="B64" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="D64" s="5">
+        <v>1</v>
+      </c>
+      <c r="E64" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F64" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="H64" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="I64" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="J64" s="5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>262</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D65" s="5">
+        <v>1</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>278</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>263</v>
+      </c>
+      <c r="H65" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="I65" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="J65" s="5" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="B66" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C64" s="5" t="s">
+      <c r="C66" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="D64" s="5">
+      <c r="D66" s="5">
         <v>2</v>
       </c>
-      <c r="E64" s="5" t="s">
+      <c r="E66" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="F64" s="5"/>
-      <c r="G64" s="5"/>
-      <c r="H64" s="5"/>
-      <c r="I64" s="5"/>
-      <c r="J64" s="5"/>
+      <c r="F66" s="5"/>
+      <c r="G66" s="5"/>
+      <c r="H66" s="5"/>
+      <c r="I66" s="5"/>
+      <c r="J66" s="5"/>
     </row>
   </sheetData>
   <sortState ref="A9:J60">

</xml_diff>

<commit_message>
add through hole parts to the bom (highlighted). update schematic pdf.
</commit_message>
<xml_diff>
--- a/pcb/labio.bom.xlsx
+++ b/pcb/labio.bom.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="316">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="336">
   <si>
     <t>Source</t>
   </si>
@@ -47,9 +47,6 @@
     <t>Title</t>
   </si>
   <si>
-    <t>Not Set</t>
-  </si>
-  <si>
     <t>Company</t>
   </si>
   <si>
@@ -975,6 +972,69 @@
   </si>
   <si>
     <t>R404, R406, R503, R512, R514</t>
+  </si>
+  <si>
+    <t>TH</t>
+  </si>
+  <si>
+    <t>Harwin, Inc.</t>
+  </si>
+  <si>
+    <t>M20-9990346</t>
+  </si>
+  <si>
+    <t>3 Positions Header, Unshrouded, Breakaway Connector 0.100" (2.54mm) Through Hole Tin</t>
+  </si>
+  <si>
+    <t>952-2264-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/harwin-inc/M20-9990346/952-2264-ND/3728228</t>
+  </si>
+  <si>
+    <t>M20-9990446</t>
+  </si>
+  <si>
+    <t>4 Positions Header, Unshrouded, Breakaway Connector 0.100" (2.54mm) Through Hole Tin</t>
+  </si>
+  <si>
+    <t>952-2266-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/harwin-inc/M20-9990446/952-2266-ND/3728230</t>
+  </si>
+  <si>
+    <t>M20-9990546</t>
+  </si>
+  <si>
+    <t>5 Positions Header, Unshrouded, Breakaway Connector 0.100" (2.54mm) Through Hole Tin</t>
+  </si>
+  <si>
+    <t>952-2268-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/harwin-inc/M20-9990546/952-2268-ND/3728232</t>
+  </si>
+  <si>
+    <t>On Shore Technology, Inc.</t>
+  </si>
+  <si>
+    <t>OSTTE020104</t>
+  </si>
+  <si>
+    <t>2 Position Wire to Board Terminal Block Horizontal with Board 0.138" (3.50mm) Through Hole</t>
+  </si>
+  <si>
+    <t>ED2740-ND</t>
+  </si>
+  <si>
+    <t>http://www.digikey.com/product-detail/en/on-shore-technology-inc/OSTTE020104/ED2740-ND/2351816</t>
+  </si>
+  <si>
+    <t>Carnegie Mellon University</t>
+  </si>
+  <si>
+    <t>Raspberry Pi Embedded Lab I/O</t>
   </si>
 </sst>
 </file>
@@ -998,12 +1058,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -1033,7 +1099,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1047,6 +1113,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1327,8 +1398,8 @@
   <dimension ref="A1:J66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B46" sqref="B46"/>
+      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1364,7 +1435,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -1372,352 +1443,352 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>335</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>6</v>
+        <v>334</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>1.2</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" t="s">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="B7" s="9">
+        <v>42606</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="D8" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="J8" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>26</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>27</v>
       </c>
       <c r="D9" s="5">
         <v>23</v>
       </c>
       <c r="E9" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="G9" s="5" t="s">
         <v>279</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="H9" s="5" t="s">
         <v>280</v>
-      </c>
-      <c r="H9" s="5" t="s">
-        <v>281</v>
       </c>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
+        <v>310</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>311</v>
       </c>
-      <c r="B10" s="5" t="s">
-        <v>312</v>
-      </c>
       <c r="C10" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D10" s="5">
         <v>1</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F10" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G10" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="H10" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="I10" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="J10" s="5" t="s">
         <v>214</v>
-      </c>
-      <c r="J10" s="5" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="D11" s="5">
         <v>10</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F11" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="G11" s="5" t="s">
         <v>211</v>
       </c>
-      <c r="G11" s="5" t="s">
+      <c r="H11" s="5" t="s">
         <v>212</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="I11" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="J11" s="5" t="s">
         <v>214</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B12" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B12" s="5" t="s">
-        <v>54</v>
-      </c>
       <c r="C12" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D12" s="5">
         <v>1</v>
       </c>
       <c r="E12" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="F12" s="5" t="s">
-        <v>279</v>
-      </c>
       <c r="G12" s="5" t="s">
+        <v>281</v>
+      </c>
+      <c r="H12" s="5" t="s">
         <v>282</v>
-      </c>
-      <c r="H12" s="5" t="s">
-        <v>283</v>
       </c>
       <c r="I12" s="5"/>
       <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
+        <v>271</v>
+      </c>
+      <c r="B13" s="5" t="s">
         <v>272</v>
       </c>
-      <c r="B13" s="5" t="s">
-        <v>273</v>
-      </c>
       <c r="C13" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D13" s="5">
         <v>1</v>
       </c>
       <c r="E13" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="F13" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="F13" s="5" t="s">
-        <v>279</v>
-      </c>
       <c r="G13" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="H13" s="5" t="s">
         <v>284</v>
-      </c>
-      <c r="H13" s="5" t="s">
-        <v>285</v>
       </c>
       <c r="I13" s="5"/>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="D14" s="5">
         <v>4</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F14" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="G14" s="5" t="s">
         <v>206</v>
       </c>
-      <c r="G14" s="5" t="s">
+      <c r="H14" s="5" t="s">
         <v>207</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="I14" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="J14" s="5" t="s">
         <v>209</v>
-      </c>
-      <c r="J14" s="5" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D15" s="5">
         <v>1</v>
       </c>
       <c r="E15" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>278</v>
       </c>
-      <c r="F15" s="5" t="s">
-        <v>279</v>
-      </c>
       <c r="G15" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="H15" s="5" t="s">
         <v>286</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>287</v>
       </c>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D16" s="5">
         <v>4</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G16" s="5" t="s">
+        <v>306</v>
+      </c>
+      <c r="H16" s="5" t="s">
         <v>307</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="I16" s="5" t="s">
         <v>308</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="J16" s="5" t="s">
         <v>309</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>310</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="B17" s="5" t="s">
         <v>252</v>
       </c>
-      <c r="B17" s="5" t="s">
-        <v>253</v>
-      </c>
       <c r="C17" s="5" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="D17" s="5">
         <v>2</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G17" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="H17" s="5" t="s">
         <v>255</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="I17" s="5" t="s">
         <v>256</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="J17" s="5" t="s">
         <v>257</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>258</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D18" s="5">
         <v>5</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
@@ -1727,179 +1798,179 @@
     </row>
     <row r="19" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="5">
         <v>19</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F19" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="G19" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="H19" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="H19" s="5" t="s">
+      <c r="I19" s="5" t="s">
         <v>179</v>
       </c>
-      <c r="I19" s="5" t="s">
+      <c r="J19" s="5" t="s">
         <v>180</v>
-      </c>
-      <c r="J19" s="5" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B20" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="C20" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="D20" s="5">
         <v>12</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F20" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="G20" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="H20" s="5" t="s">
         <v>142</v>
       </c>
-      <c r="H20" s="5" t="s">
+      <c r="I20" s="5" t="s">
         <v>143</v>
       </c>
-      <c r="I20" s="5" t="s">
+      <c r="J20" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D21" s="5">
         <v>6</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="H21" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="I21" s="5" t="s">
         <v>243</v>
       </c>
-      <c r="I21" s="5" t="s">
+      <c r="J21" s="5" t="s">
         <v>244</v>
-      </c>
-      <c r="J21" s="5" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B22" s="5" t="s">
         <v>235</v>
       </c>
-      <c r="B22" s="5" t="s">
-        <v>236</v>
-      </c>
       <c r="C22" s="5" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D22" s="5">
         <v>1</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F22" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="G22" s="5" t="s">
         <v>238</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="H22" s="5" t="s">
         <v>239</v>
       </c>
-      <c r="H22" s="5" t="s">
+      <c r="I22" s="5" t="s">
         <v>240</v>
       </c>
-      <c r="I22" s="5" t="s">
+      <c r="J22" s="5" t="s">
         <v>241</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D23" s="5">
         <v>1</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F23" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="G23" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="H23" s="5" t="s">
         <v>248</v>
       </c>
-      <c r="H23" s="5" t="s">
+      <c r="I23" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="I23" s="5" t="s">
+      <c r="J23" s="5" t="s">
         <v>250</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="C24" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>105</v>
-      </c>
       <c r="D24" s="5">
         <v>1</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F24" s="5"/>
       <c r="G24" s="5"/>
@@ -1909,19 +1980,19 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="B25" s="5" t="s">
+      <c r="C25" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>100</v>
-      </c>
       <c r="D25" s="5">
         <v>1</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F25" s="5"/>
       <c r="G25" s="5"/>
@@ -1931,19 +2002,19 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B26" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>107</v>
-      </c>
       <c r="D26" s="5">
         <v>1</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F26" s="5"/>
       <c r="G26" s="5"/>
@@ -1953,19 +2024,19 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="C27" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B27" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>102</v>
-      </c>
       <c r="D27" s="5">
         <v>1</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F27" s="5"/>
       <c r="G27" s="5"/>
@@ -1975,19 +2046,19 @@
     </row>
     <row r="28" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>96</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>97</v>
       </c>
       <c r="D28" s="5">
         <v>9</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5"/>
@@ -1997,19 +2068,19 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C29" s="5" t="s">
-        <v>17</v>
-      </c>
       <c r="D29" s="5">
         <v>1</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
@@ -2019,51 +2090,51 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="B30" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="C30" s="5" t="s">
-        <v>81</v>
-      </c>
       <c r="D30" s="5">
         <v>1</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F30" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="G30" s="5" t="s">
         <v>162</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="H30" s="5" t="s">
         <v>163</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="I30" s="5" t="s">
         <v>164</v>
       </c>
-      <c r="I30" s="5" t="s">
+      <c r="J30" s="5" t="s">
         <v>165</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C31" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="D31" s="5">
         <v>1</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
@@ -2072,140 +2143,180 @@
       <c r="J31" s="5"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="B32" s="5" t="s">
+      <c r="A32" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C32" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="5">
+      <c r="D32" s="8">
         <v>7</v>
       </c>
-      <c r="E32" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="5"/>
+      <c r="E32" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="G32" s="8" t="s">
+        <v>321</v>
+      </c>
+      <c r="H32" s="8" t="s">
+        <v>322</v>
+      </c>
+      <c r="I32" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="J32" s="8" t="s">
+        <v>324</v>
+      </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="C33" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C33" s="5" t="s">
-        <v>43</v>
-      </c>
       <c r="D33" s="5">
         <v>1</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F33" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="G33" s="5" t="s">
         <v>172</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>173</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="I33" s="5" t="s">
         <v>174</v>
       </c>
-      <c r="I33" s="5" t="s">
+      <c r="J33" s="5" t="s">
         <v>175</v>
       </c>
-      <c r="J33" s="5" t="s">
-        <v>176</v>
-      </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" s="8">
+        <v>1</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="G34" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="J34" s="8" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A35" s="7" t="s">
         <v>123</v>
       </c>
-      <c r="B34" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="D34" s="5">
-        <v>1</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F34" s="5"/>
-      <c r="G34" s="5"/>
-      <c r="H34" s="5"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="5"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B35" s="5" t="s">
+      <c r="B35" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C35" s="5" t="s">
+      <c r="D35" s="8">
+        <v>2</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="F35" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="G35" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="H35" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="J35" s="8" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A36" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="B36" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="D35" s="5">
+      <c r="C36" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="D36" s="8">
         <v>2</v>
       </c>
-      <c r="E35" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F35" s="5"/>
-      <c r="G35" s="5"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" s="5">
-        <v>2</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F36" s="5"/>
-      <c r="G36" s="5"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
+      <c r="E36" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="F36" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="G36" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="H36" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="I36" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="J36" s="8" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C37" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="B37" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C37" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="D37" s="5">
         <v>1</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
@@ -2215,19 +2326,19 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B38" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B38" s="5" t="s">
+      <c r="C38" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C38" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="D38" s="5">
         <v>1</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
@@ -2237,111 +2348,111 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="B39" s="5" t="s">
+      <c r="C39" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="C39" s="5" t="s">
-        <v>35</v>
-      </c>
       <c r="D39" s="5">
         <v>1</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F39" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="G39" s="5" t="s">
         <v>157</v>
       </c>
-      <c r="G39" s="5" t="s">
+      <c r="H39" s="5" t="s">
         <v>158</v>
       </c>
-      <c r="H39" s="5" t="s">
+      <c r="I39" s="5" t="s">
         <v>159</v>
       </c>
-      <c r="I39" s="5" t="s">
+      <c r="J39" s="5" t="s">
         <v>160</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B40" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="5" t="s">
         <v>39</v>
-      </c>
-      <c r="C40" s="5" t="s">
-        <v>40</v>
       </c>
       <c r="D40" s="5">
         <v>15</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F40" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="G40" s="5" t="s">
         <v>201</v>
       </c>
-      <c r="G40" s="5" t="s">
+      <c r="H40" s="5" t="s">
         <v>202</v>
       </c>
-      <c r="H40" s="5" t="s">
+      <c r="I40" s="5" t="s">
         <v>203</v>
       </c>
-      <c r="I40" s="5" t="s">
+      <c r="J40" s="5" t="s">
         <v>204</v>
-      </c>
-      <c r="J40" s="5" t="s">
-        <v>205</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C41" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D41" s="5">
         <v>4</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F41" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="G41" s="5" t="s">
         <v>288</v>
       </c>
-      <c r="G41" s="5" t="s">
+      <c r="H41" s="5" t="s">
         <v>289</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>290</v>
       </c>
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C42" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D42" s="5">
         <v>1</v>
       </c>
       <c r="E42" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
@@ -2351,19 +2462,19 @@
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D43" s="5">
         <v>2</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F43" s="5"/>
       <c r="G43" s="5"/>
@@ -2373,689 +2484,689 @@
     </row>
     <row r="44" spans="1:10" ht="48" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B44" s="5">
         <v>220</v>
       </c>
       <c r="C44" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D44" s="5">
         <v>19</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G44" s="5" t="s">
+        <v>290</v>
+      </c>
+      <c r="H44" s="5" t="s">
         <v>291</v>
-      </c>
-      <c r="H44" s="5" t="s">
-        <v>292</v>
       </c>
       <c r="I44" s="5"/>
       <c r="J44" s="5"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B45" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="5" t="s">
         <v>19</v>
-      </c>
-      <c r="C45" s="5" t="s">
-        <v>20</v>
       </c>
       <c r="D45" s="5">
         <v>7</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G45" s="5" t="s">
+        <v>292</v>
+      </c>
+      <c r="H45" s="5" t="s">
         <v>293</v>
-      </c>
-      <c r="H45" s="5" t="s">
-        <v>294</v>
       </c>
       <c r="I45" s="5"/>
       <c r="J45" s="5"/>
     </row>
     <row r="46" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B46" s="5">
         <v>0</v>
       </c>
       <c r="C46" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D46" s="5">
         <v>13</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G46" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="H46" s="5" t="s">
         <v>295</v>
-      </c>
-      <c r="H46" s="5" t="s">
-        <v>296</v>
       </c>
       <c r="I46" s="5"/>
       <c r="J46" s="5"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C47" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D47" s="5">
         <v>5</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G47" s="5" t="s">
+        <v>294</v>
+      </c>
+      <c r="H47" s="5" t="s">
         <v>295</v>
-      </c>
-      <c r="H47" s="5" t="s">
-        <v>296</v>
       </c>
       <c r="I47" s="5"/>
       <c r="J47" s="5"/>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
+        <v>312</v>
+      </c>
+      <c r="B48" s="5" t="s">
         <v>313</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>314</v>
-      </c>
       <c r="C48" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D48" s="5">
         <v>1</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G48" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="H48" s="5" t="s">
         <v>299</v>
-      </c>
-      <c r="H48" s="5" t="s">
-        <v>300</v>
       </c>
       <c r="I48" s="5"/>
       <c r="J48" s="5"/>
     </row>
     <row r="49" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C49" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D49" s="5">
         <v>15</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G49" s="5" t="s">
+        <v>296</v>
+      </c>
+      <c r="H49" s="5" t="s">
         <v>297</v>
-      </c>
-      <c r="H49" s="5" t="s">
-        <v>298</v>
       </c>
       <c r="I49" s="5"/>
       <c r="J49" s="5"/>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B50" s="5">
         <v>0.01</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D50" s="5">
         <v>2</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="G50" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="H50" s="5" t="s">
         <v>303</v>
       </c>
-      <c r="H50" s="5" t="s">
+      <c r="I50" s="5" t="s">
         <v>304</v>
       </c>
-      <c r="I50" s="5" t="s">
+      <c r="J50" s="5" t="s">
         <v>305</v>
-      </c>
-      <c r="J50" s="5" t="s">
-        <v>306</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B51" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="B51" s="5" t="s">
-        <v>88</v>
-      </c>
       <c r="C51" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D51" s="5">
         <v>1</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G51" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="H51" s="5" t="s">
         <v>299</v>
-      </c>
-      <c r="H51" s="5" t="s">
-        <v>300</v>
       </c>
       <c r="I51" s="5"/>
       <c r="J51" s="5"/>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B52" s="5" t="s">
         <v>268</v>
       </c>
-      <c r="B52" s="5" t="s">
-        <v>269</v>
-      </c>
       <c r="C52" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D52" s="5">
         <v>1</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G52" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="H52" s="5" t="s">
         <v>301</v>
-      </c>
-      <c r="H52" s="5" t="s">
-        <v>302</v>
       </c>
       <c r="I52" s="5"/>
       <c r="J52" s="5"/>
     </row>
     <row r="53" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B53" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C53" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="C53" s="5" t="s">
-        <v>37</v>
       </c>
       <c r="D53" s="5">
         <v>10</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F53" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="G53" s="5" t="s">
         <v>167</v>
       </c>
-      <c r="G53" s="5" t="s">
+      <c r="H53" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="H53" s="5" t="s">
+      <c r="I53" s="5" t="s">
         <v>169</v>
       </c>
-      <c r="I53" s="5" t="s">
+      <c r="J53" s="5" t="s">
         <v>170</v>
       </c>
-      <c r="J53" s="5" t="s">
-        <v>171</v>
-      </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A54" s="4" t="s">
+      <c r="A54" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B54" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="C54" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="C54" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="D54" s="5">
-        <v>1</v>
-      </c>
-      <c r="E54" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="F54" s="5" t="s">
+      <c r="D54" s="8">
+        <v>1</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="F54" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="G54" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="G54" s="5" t="s">
+      <c r="H54" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="H54" s="5" t="s">
+      <c r="I54" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="I54" s="5" t="s">
+      <c r="J54" s="8" t="s">
         <v>233</v>
-      </c>
-      <c r="J54" s="5" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B55" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="C55" s="5" t="s">
         <v>90</v>
-      </c>
-      <c r="C55" s="5" t="s">
-        <v>91</v>
       </c>
       <c r="D55" s="5">
         <v>5</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F55" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="G55" s="5" t="s">
         <v>146</v>
       </c>
-      <c r="G55" s="5" t="s">
+      <c r="H55" s="5" t="s">
         <v>147</v>
       </c>
-      <c r="H55" s="5" t="s">
+      <c r="I55" s="5" t="s">
         <v>148</v>
       </c>
-      <c r="I55" s="5" t="s">
+      <c r="J55" s="5" t="s">
         <v>149</v>
-      </c>
-      <c r="J55" s="5" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B56" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B56" s="5" t="s">
+      <c r="C56" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="C56" s="5" t="s">
-        <v>25</v>
-      </c>
       <c r="D56" s="5">
         <v>1</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F56" s="5" t="s">
+        <v>134</v>
+      </c>
+      <c r="G56" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="G56" s="5" t="s">
+      <c r="H56" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="I56" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="H56" s="5" t="s">
-        <v>140</v>
-      </c>
-      <c r="I56" s="5" t="s">
+      <c r="J56" s="5" t="s">
         <v>137</v>
-      </c>
-      <c r="J56" s="5" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B57" s="5" t="s">
+      <c r="C57" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C57" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="D57" s="5">
         <v>1</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F57" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G57" s="5" t="s">
         <v>152</v>
       </c>
-      <c r="G57" s="5" t="s">
+      <c r="H57" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="I57" s="5" t="s">
         <v>153</v>
       </c>
-      <c r="H57" s="5" t="s">
+      <c r="J57" s="5" t="s">
         <v>155</v>
-      </c>
-      <c r="I57" s="5" t="s">
-        <v>154</v>
-      </c>
-      <c r="J57" s="5" t="s">
-        <v>156</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C58" s="5"/>
       <c r="D58" s="5">
         <v>1</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F58" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="G58" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="H58" s="5" t="s">
         <v>227</v>
       </c>
-      <c r="G58" s="5" t="s">
-        <v>226</v>
-      </c>
-      <c r="H58" s="5" t="s">
+      <c r="I58" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="J58" s="5" t="s">
         <v>228</v>
-      </c>
-      <c r="I58" s="5" t="s">
-        <v>217</v>
-      </c>
-      <c r="J58" s="5" t="s">
-        <v>229</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B59" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="C59" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>48</v>
-      </c>
       <c r="D59" s="5">
         <v>1</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G59" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="H59" s="5" t="s">
         <v>196</v>
       </c>
-      <c r="H59" s="5" t="s">
+      <c r="I59" s="5" t="s">
         <v>197</v>
       </c>
-      <c r="I59" s="5" t="s">
+      <c r="J59" s="5" t="s">
         <v>198</v>
-      </c>
-      <c r="J59" s="5" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B60" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B60" s="5" t="s">
+      <c r="C60" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="C60" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="D60" s="5">
         <v>1</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="H60" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="I60" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J60" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B61" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B61" s="5" t="s">
-        <v>56</v>
-      </c>
       <c r="C61" s="5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D61" s="5">
         <v>1</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G61" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="H61" s="5" t="s">
         <v>192</v>
       </c>
-      <c r="H61" s="5" t="s">
+      <c r="I61" s="5" t="s">
         <v>193</v>
       </c>
-      <c r="I61" s="5" t="s">
+      <c r="J61" s="5" t="s">
         <v>194</v>
-      </c>
-      <c r="J61" s="5" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B62" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="B62" s="5" t="s">
+      <c r="C62" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C62" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="D62" s="5">
         <v>1</v>
       </c>
       <c r="E62" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F62" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="G62" s="5" t="s">
         <v>187</v>
       </c>
-      <c r="G62" s="5" t="s">
+      <c r="H62" s="5" t="s">
         <v>188</v>
       </c>
-      <c r="H62" s="5" t="s">
+      <c r="I62" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="I62" s="5" t="s">
+      <c r="J62" s="5" t="s">
         <v>190</v>
-      </c>
-      <c r="J62" s="5" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B63" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="C63" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C63" s="5" t="s">
-        <v>84</v>
-      </c>
       <c r="D63" s="5">
         <v>1</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F63" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="G63" s="5" t="s">
         <v>182</v>
       </c>
-      <c r="G63" s="5" t="s">
+      <c r="H63" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="I63" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="H63" s="5" t="s">
+      <c r="J63" s="5" t="s">
         <v>185</v>
-      </c>
-      <c r="I63" s="5" t="s">
-        <v>184</v>
-      </c>
-      <c r="J63" s="5" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="C64" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B64" s="5" t="s">
-        <v>220</v>
-      </c>
-      <c r="C64" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="D64" s="5">
         <v>1</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G64" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="H64" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="H64" s="5" t="s">
+      <c r="I64" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="I64" s="5" t="s">
+      <c r="J64" s="5" t="s">
         <v>224</v>
-      </c>
-      <c r="J64" s="5" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="B65" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="B65" s="5" t="s">
+      <c r="C65" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D65" s="5">
+        <v>1</v>
+      </c>
+      <c r="E65" s="5" t="s">
+        <v>277</v>
+      </c>
+      <c r="F65" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="G65" s="5" t="s">
         <v>262</v>
       </c>
-      <c r="C65" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D65" s="5">
-        <v>1</v>
-      </c>
-      <c r="E65" s="5" t="s">
-        <v>278</v>
-      </c>
-      <c r="F65" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="G65" s="5" t="s">
+      <c r="H65" s="5" t="s">
         <v>263</v>
       </c>
-      <c r="H65" s="5" t="s">
+      <c r="I65" s="5" t="s">
         <v>264</v>
       </c>
-      <c r="I65" s="5" t="s">
+      <c r="J65" s="5" t="s">
         <v>265</v>
-      </c>
-      <c r="J65" s="5" t="s">
-        <v>266</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B66" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C66" s="5" t="s">
         <v>21</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>22</v>
       </c>
       <c r="D66" s="5">
         <v>2</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F66" s="5"/>
       <c r="G66" s="5"/>

</xml_diff>

<commit_message>
fix bom qty for P601 P602 P604 (screw in header)
</commit_message>
<xml_diff>
--- a/pcb/labio.bom.xlsx
+++ b/pcb/labio.bom.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27309"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="460" windowWidth="21740" windowHeight="20540" tabRatio="500"/>
+    <workbookView xWindow="31660" yWindow="-180" windowWidth="21740" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="labio.bom" sheetId="1" r:id="rId1"/>
@@ -1099,7 +1099,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1118,6 +1118,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1398,8 +1402,8 @@
   <dimension ref="A1:J66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="8" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="8" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2143,162 +2147,162 @@
       <c r="J31" s="5"/>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A32" s="7" t="s">
+      <c r="A32" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="C32" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="D32" s="8">
+      <c r="D32" s="11">
         <v>7</v>
       </c>
-      <c r="E32" s="8" t="s">
+      <c r="E32" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="F32" s="8" t="s">
+      <c r="F32" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="G32" s="8" t="s">
+      <c r="G32" s="11" t="s">
         <v>321</v>
       </c>
-      <c r="H32" s="8" t="s">
+      <c r="H32" s="11" t="s">
         <v>322</v>
       </c>
-      <c r="I32" s="8" t="s">
+      <c r="I32" s="11" t="s">
         <v>323</v>
       </c>
-      <c r="J32" s="8" t="s">
+      <c r="J32" s="11" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
+      <c r="A33" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D33" s="5">
-        <v>1</v>
-      </c>
-      <c r="E33" s="5" t="s">
-        <v>277</v>
-      </c>
-      <c r="F33" s="5" t="s">
+      <c r="D33" s="11">
+        <v>1</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>277</v>
+      </c>
+      <c r="F33" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="G33" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="H33" s="5" t="s">
+      <c r="H33" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="I33" s="5" t="s">
+      <c r="I33" s="11" t="s">
         <v>174</v>
       </c>
-      <c r="J33" s="5" t="s">
+      <c r="J33" s="11" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A34" s="7" t="s">
+      <c r="A34" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="B34" s="8" t="s">
+      <c r="B34" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="C34" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D34" s="8">
-        <v>1</v>
-      </c>
-      <c r="E34" s="8" t="s">
+      <c r="D34" s="11">
+        <v>3</v>
+      </c>
+      <c r="E34" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="F34" s="8" t="s">
+      <c r="F34" s="11" t="s">
         <v>329</v>
       </c>
-      <c r="G34" s="8" t="s">
+      <c r="G34" s="11" t="s">
         <v>330</v>
       </c>
-      <c r="H34" s="8" t="s">
+      <c r="H34" s="11" t="s">
         <v>331</v>
       </c>
-      <c r="I34" s="8" t="s">
+      <c r="I34" s="11" t="s">
         <v>332</v>
       </c>
-      <c r="J34" s="8" t="s">
+      <c r="J34" s="11" t="s">
         <v>333</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A35" s="7" t="s">
+      <c r="A35" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D35" s="11">
         <v>2</v>
       </c>
-      <c r="E35" s="8" t="s">
+      <c r="E35" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="F35" s="8" t="s">
+      <c r="F35" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="G35" s="8" t="s">
+      <c r="G35" s="11" t="s">
         <v>317</v>
       </c>
-      <c r="H35" s="8" t="s">
+      <c r="H35" s="11" t="s">
         <v>318</v>
       </c>
-      <c r="I35" s="8" t="s">
+      <c r="I35" s="11" t="s">
         <v>319</v>
       </c>
-      <c r="J35" s="8" t="s">
+      <c r="J35" s="11" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A36" s="7" t="s">
+      <c r="A36" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="B36" s="8" t="s">
+      <c r="B36" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="C36" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D36" s="11">
         <v>2</v>
       </c>
-      <c r="E36" s="8" t="s">
+      <c r="E36" s="11" t="s">
         <v>315</v>
       </c>
-      <c r="F36" s="8" t="s">
+      <c r="F36" s="11" t="s">
         <v>316</v>
       </c>
-      <c r="G36" s="8" t="s">
+      <c r="G36" s="11" t="s">
         <v>325</v>
       </c>
-      <c r="H36" s="8" t="s">
+      <c r="H36" s="11" t="s">
         <v>326</v>
       </c>
-      <c r="I36" s="8" t="s">
+      <c r="I36" s="11" t="s">
         <v>327</v>
       </c>
-      <c r="J36" s="8" t="s">
+      <c r="J36" s="11" t="s">
         <v>328</v>
       </c>
     </row>

</xml_diff>